<commit_message>
fixed #189 FlixelRL-189 レベル作成(Floor:1〜3)
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="382">
   <si>
     <t>id</t>
   </si>
@@ -1114,6 +1114,9 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>item</t>
   </si>
   <si>
     <t>cnt</t>
@@ -1197,7 +1200,7 @@
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1213,6 +1216,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1246,7 +1291,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1274,6 +1319,51 @@
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1293,6 +1383,13 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffd478"/>
+      <rgbColor rgb="ffd4fb78"/>
+      <rgbColor rgb="ff72fcd5"/>
+      <rgbColor rgb="ff75d5ff"/>
+      <rgbColor rgb="ffd783ff"/>
+      <rgbColor rgb="ffff89d8"/>
+      <rgbColor rgb="ffff2f92"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -7639,7 +7736,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -7648,18 +7745,19 @@
     <col min="1" max="1" width="2.5" style="8" customWidth="1"/>
     <col min="2" max="2" width="4" style="8" customWidth="1"/>
     <col min="3" max="3" width="4.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="3.25" style="8" customWidth="1"/>
-    <col min="6" max="6" width="3.625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.75" style="8" customWidth="1"/>
-    <col min="8" max="8" width="3.625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="3.625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="2.375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="3.625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="2.375" style="8" customWidth="1"/>
-    <col min="14" max="14" width="3.625" style="8" customWidth="1"/>
-    <col min="15" max="256" width="12.25" style="8" customWidth="1"/>
+    <col min="4" max="4" width="3.625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="2.875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="3.25" style="8" customWidth="1"/>
+    <col min="7" max="7" width="3.625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.75" style="8" customWidth="1"/>
+    <col min="9" max="9" width="3.625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="3.125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="3.625" style="8" customWidth="1"/>
+    <col min="12" max="12" width="2.375" style="8" customWidth="1"/>
+    <col min="13" max="13" width="3.625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="2.375" style="8" customWidth="1"/>
+    <col min="15" max="15" width="3.625" style="8" customWidth="1"/>
+    <col min="16" max="256" width="12.25" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -7705,48 +7803,54 @@
       <c r="N1" t="s" s="2">
         <v>377</v>
       </c>
+      <c r="O1" t="s" s="2">
+        <v>378</v>
+      </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
       <c r="A2" t="s" s="4">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="C2" t="s" s="5">
+      <c r="C2" t="s" s="9">
         <v>10</v>
       </c>
-      <c r="D2" t="s" s="5">
+      <c r="D2" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="E2" t="s" s="5">
+      <c r="E2" t="s" s="10">
         <v>10</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="F2" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="G2" t="s" s="11">
         <v>10</v>
       </c>
-      <c r="H2" t="s" s="5">
+      <c r="H2" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="I2" t="s" s="5">
+      <c r="I2" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="J2" t="s" s="5">
+      <c r="J2" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="5">
+      <c r="K2" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="L2" t="s" s="5">
+      <c r="L2" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="M2" t="s" s="5">
+      <c r="M2" t="s" s="14">
         <v>10</v>
       </c>
-      <c r="N2" t="s" s="5">
+      <c r="N2" t="s" s="15">
+        <v>10</v>
+      </c>
+      <c r="O2" t="s" s="15">
         <v>10</v>
       </c>
     </row>
@@ -7754,187 +7858,181 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10">
         <v>2</v>
       </c>
-      <c r="E3" t="s" s="5">
-        <v>378</v>
-      </c>
-      <c r="F3" s="6">
-        <v>100</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="9">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="5">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s" s="5">
-        <v>378</v>
-      </c>
-      <c r="F4" s="6">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s" s="5">
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s" s="11">
         <v>379</v>
       </c>
-      <c r="H4" s="6">
-        <v>100</v>
-      </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="G4" s="17">
+        <v>100</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
-        <f>C4+1</f>
-        <v>4</v>
-      </c>
-      <c r="C5" s="5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s" s="5">
-        <v>378</v>
-      </c>
-      <c r="F5" s="6">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s" s="5">
+      <c r="B5" s="9">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s" s="11">
         <v>379</v>
       </c>
-      <c r="H5" s="6">
-        <v>100</v>
-      </c>
-      <c r="I5" t="s" s="5">
+      <c r="G5" s="17">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s" s="12">
         <v>380</v>
       </c>
-      <c r="J5" s="6">
-        <v>100</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="I5" s="18">
+        <v>100</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
-        <f>C5+1</f>
-        <v>7</v>
-      </c>
-      <c r="C6" s="5">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="6">
-        <v>100</v>
-      </c>
-      <c r="G6" s="6">
+      <c r="B6" s="9">
+        <f>C4+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="9">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10">
         <v>2</v>
       </c>
-      <c r="H6" s="6">
-        <v>100</v>
-      </c>
-      <c r="I6" s="6">
-        <v>3</v>
-      </c>
-      <c r="J6" s="6">
-        <v>100</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="E6" s="10">
         <v>4</v>
       </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>5</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
+      <c r="F6" t="s" s="11">
+        <v>379</v>
+      </c>
+      <c r="G6" s="17">
+        <v>25</v>
+      </c>
+      <c r="H6" t="s" s="12">
+        <v>380</v>
+      </c>
+      <c r="I6" s="18">
+        <v>100</v>
+      </c>
+      <c r="J6" t="s" s="13">
+        <v>381</v>
+      </c>
+      <c r="K6" s="19">
+        <v>100</v>
+      </c>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="9">
         <f>C6+1</f>
-        <v>11</v>
-      </c>
-      <c r="C7" s="5">
-        <v>15</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
-        <v>1</v>
-      </c>
-      <c r="F7" s="6">
-        <v>100</v>
-      </c>
-      <c r="G7" s="6">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10">
         <v>2</v>
       </c>
-      <c r="H7" s="6">
-        <v>100</v>
-      </c>
-      <c r="I7" s="6">
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1</v>
+      </c>
+      <c r="G7" s="17">
+        <v>100</v>
+      </c>
+      <c r="H7" s="18">
+        <v>2</v>
+      </c>
+      <c r="I7" s="18">
+        <v>100</v>
+      </c>
+      <c r="J7" s="19">
         <v>3</v>
       </c>
-      <c r="J7" s="6">
-        <v>100</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="K7" s="19">
+        <v>100</v>
+      </c>
+      <c r="L7" s="20">
         <v>4</v>
       </c>
-      <c r="L7" s="6">
+      <c r="M7" s="20">
         <v>0</v>
       </c>
-      <c r="M7" s="6">
+      <c r="N7" s="21">
         <v>5</v>
       </c>
-      <c r="N7" s="6">
+      <c r="O7" s="21">
         <v>0</v>
       </c>
     </row>
@@ -7942,44 +8040,47 @@
       <c r="A8" s="4">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <f>C7+1</f>
-        <v>16</v>
-      </c>
-      <c r="C8" s="5">
-        <v>20</v>
-      </c>
-      <c r="D8" s="5">
-        <v>1</v>
-      </c>
-      <c r="E8" s="5">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>100</v>
-      </c>
-      <c r="G8" s="6">
+        <v>11</v>
+      </c>
+      <c r="C8" s="9">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="6">
-        <v>100</v>
-      </c>
-      <c r="I8" s="6">
+      <c r="E8" s="10">
+        <v>1</v>
+      </c>
+      <c r="F8" s="11">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17">
+        <v>100</v>
+      </c>
+      <c r="H8" s="18">
+        <v>2</v>
+      </c>
+      <c r="I8" s="18">
+        <v>100</v>
+      </c>
+      <c r="J8" s="19">
         <v>3</v>
       </c>
-      <c r="J8" s="6">
-        <v>100</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="K8" s="19">
+        <v>100</v>
+      </c>
+      <c r="L8" s="20">
         <v>4</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="20">
         <v>0</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="21">
         <v>5</v>
       </c>
-      <c r="N8" s="6">
+      <c r="O8" s="21">
         <v>0</v>
       </c>
     </row>
@@ -7987,44 +8088,47 @@
       <c r="A9" s="4">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <f>C8+1</f>
-        <v>21</v>
-      </c>
-      <c r="C9" s="5">
-        <v>30</v>
-      </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6">
-        <v>100</v>
-      </c>
-      <c r="G9" s="6">
+        <v>16</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
         <v>2</v>
       </c>
-      <c r="H9" s="6">
-        <v>100</v>
-      </c>
-      <c r="I9" s="6">
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="11">
+        <v>1</v>
+      </c>
+      <c r="G9" s="17">
+        <v>100</v>
+      </c>
+      <c r="H9" s="18">
+        <v>2</v>
+      </c>
+      <c r="I9" s="18">
+        <v>100</v>
+      </c>
+      <c r="J9" s="19">
         <v>3</v>
       </c>
-      <c r="J9" s="6">
-        <v>100</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="K9" s="19">
+        <v>100</v>
+      </c>
+      <c r="L9" s="20">
         <v>4</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="20">
         <v>0</v>
       </c>
-      <c r="M9" s="6">
+      <c r="N9" s="21">
         <v>5</v>
       </c>
-      <c r="N9" s="6">
+      <c r="O9" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8032,44 +8136,47 @@
       <c r="A10" s="4">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="9">
         <f>C9+1</f>
-        <v>31</v>
-      </c>
-      <c r="C10" s="5">
-        <v>40</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1</v>
-      </c>
-      <c r="F10" s="6">
-        <v>100</v>
-      </c>
-      <c r="G10" s="6">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>30</v>
+      </c>
+      <c r="D10" s="10">
         <v>2</v>
       </c>
-      <c r="H10" s="6">
-        <v>100</v>
-      </c>
-      <c r="I10" s="6">
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17">
+        <v>100</v>
+      </c>
+      <c r="H10" s="18">
+        <v>2</v>
+      </c>
+      <c r="I10" s="18">
+        <v>100</v>
+      </c>
+      <c r="J10" s="19">
         <v>3</v>
       </c>
-      <c r="J10" s="6">
-        <v>100</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="K10" s="19">
+        <v>100</v>
+      </c>
+      <c r="L10" s="20">
         <v>4</v>
       </c>
-      <c r="L10" s="6">
+      <c r="M10" s="20">
         <v>0</v>
       </c>
-      <c r="M10" s="6">
+      <c r="N10" s="21">
         <v>5</v>
       </c>
-      <c r="N10" s="6">
+      <c r="O10" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8077,44 +8184,47 @@
       <c r="A11" s="4">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="9">
         <f>C10+1</f>
-        <v>41</v>
-      </c>
-      <c r="C11" s="5">
-        <v>60</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6">
-        <v>100</v>
-      </c>
-      <c r="G11" s="6">
+        <v>31</v>
+      </c>
+      <c r="C11" s="9">
+        <v>40</v>
+      </c>
+      <c r="D11" s="10">
         <v>2</v>
       </c>
-      <c r="H11" s="6">
-        <v>100</v>
-      </c>
-      <c r="I11" s="6">
+      <c r="E11" s="10">
+        <v>1</v>
+      </c>
+      <c r="F11" s="11">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17">
+        <v>100</v>
+      </c>
+      <c r="H11" s="18">
+        <v>2</v>
+      </c>
+      <c r="I11" s="18">
+        <v>100</v>
+      </c>
+      <c r="J11" s="19">
         <v>3</v>
       </c>
-      <c r="J11" s="6">
-        <v>100</v>
-      </c>
-      <c r="K11" s="6">
+      <c r="K11" s="19">
+        <v>100</v>
+      </c>
+      <c r="L11" s="20">
         <v>4</v>
       </c>
-      <c r="L11" s="6">
+      <c r="M11" s="20">
         <v>0</v>
       </c>
-      <c r="M11" s="6">
+      <c r="N11" s="21">
         <v>5</v>
       </c>
-      <c r="N11" s="6">
+      <c r="O11" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8122,44 +8232,47 @@
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="9">
         <f>C11+1</f>
-        <v>61</v>
-      </c>
-      <c r="C12" s="5">
-        <v>80</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6">
-        <v>100</v>
-      </c>
-      <c r="G12" s="6">
+        <v>41</v>
+      </c>
+      <c r="C12" s="9">
+        <v>60</v>
+      </c>
+      <c r="D12" s="10">
         <v>2</v>
       </c>
-      <c r="H12" s="6">
-        <v>100</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17">
+        <v>100</v>
+      </c>
+      <c r="H12" s="18">
+        <v>2</v>
+      </c>
+      <c r="I12" s="18">
+        <v>100</v>
+      </c>
+      <c r="J12" s="19">
         <v>3</v>
       </c>
-      <c r="J12" s="6">
-        <v>100</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="K12" s="19">
+        <v>100</v>
+      </c>
+      <c r="L12" s="20">
         <v>4</v>
       </c>
-      <c r="L12" s="6">
+      <c r="M12" s="20">
         <v>0</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N12" s="21">
         <v>5</v>
       </c>
-      <c r="N12" s="6">
+      <c r="O12" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8167,44 +8280,47 @@
       <c r="A13" s="4">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="9">
         <f>C12+1</f>
-        <v>81</v>
-      </c>
-      <c r="C13" s="5">
-        <v>100</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6">
-        <v>100</v>
-      </c>
-      <c r="G13" s="6">
+        <v>61</v>
+      </c>
+      <c r="C13" s="9">
+        <v>80</v>
+      </c>
+      <c r="D13" s="10">
         <v>2</v>
       </c>
-      <c r="H13" s="6">
-        <v>100</v>
-      </c>
-      <c r="I13" s="6">
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="17">
+        <v>100</v>
+      </c>
+      <c r="H13" s="18">
+        <v>2</v>
+      </c>
+      <c r="I13" s="18">
+        <v>100</v>
+      </c>
+      <c r="J13" s="19">
         <v>3</v>
       </c>
-      <c r="J13" s="6">
-        <v>100</v>
-      </c>
-      <c r="K13" s="6">
+      <c r="K13" s="19">
+        <v>100</v>
+      </c>
+      <c r="L13" s="20">
         <v>4</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="20">
         <v>0</v>
       </c>
-      <c r="M13" s="6">
+      <c r="N13" s="21">
         <v>5</v>
       </c>
-      <c r="N13" s="6">
+      <c r="O13" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8212,44 +8328,47 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="9">
         <f>C13+1</f>
-        <v>101</v>
-      </c>
-      <c r="C14" s="5">
-        <v>150</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5">
-        <v>1</v>
-      </c>
-      <c r="F14" s="6">
-        <v>100</v>
-      </c>
-      <c r="G14" s="6">
+        <v>81</v>
+      </c>
+      <c r="C14" s="9">
+        <v>100</v>
+      </c>
+      <c r="D14" s="10">
         <v>2</v>
       </c>
-      <c r="H14" s="6">
-        <v>100</v>
-      </c>
-      <c r="I14" s="6">
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17">
+        <v>100</v>
+      </c>
+      <c r="H14" s="18">
+        <v>2</v>
+      </c>
+      <c r="I14" s="18">
+        <v>100</v>
+      </c>
+      <c r="J14" s="19">
         <v>3</v>
       </c>
-      <c r="J14" s="6">
-        <v>100</v>
-      </c>
-      <c r="K14" s="6">
+      <c r="K14" s="19">
+        <v>100</v>
+      </c>
+      <c r="L14" s="20">
         <v>4</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="20">
         <v>0</v>
       </c>
-      <c r="M14" s="6">
+      <c r="N14" s="21">
         <v>5</v>
       </c>
-      <c r="N14" s="6">
+      <c r="O14" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8257,44 +8376,47 @@
       <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="9">
         <f>C14+1</f>
-        <v>151</v>
-      </c>
-      <c r="C15" s="5">
-        <v>200</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>1</v>
-      </c>
-      <c r="F15" s="6">
-        <v>100</v>
-      </c>
-      <c r="G15" s="6">
+        <v>101</v>
+      </c>
+      <c r="C15" s="9">
+        <v>150</v>
+      </c>
+      <c r="D15" s="10">
         <v>2</v>
       </c>
-      <c r="H15" s="6">
-        <v>100</v>
-      </c>
-      <c r="I15" s="6">
+      <c r="E15" s="10">
+        <v>1</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1</v>
+      </c>
+      <c r="G15" s="17">
+        <v>100</v>
+      </c>
+      <c r="H15" s="18">
+        <v>2</v>
+      </c>
+      <c r="I15" s="18">
+        <v>100</v>
+      </c>
+      <c r="J15" s="19">
         <v>3</v>
       </c>
-      <c r="J15" s="6">
-        <v>100</v>
-      </c>
-      <c r="K15" s="6">
+      <c r="K15" s="19">
+        <v>100</v>
+      </c>
+      <c r="L15" s="20">
         <v>4</v>
       </c>
-      <c r="L15" s="6">
+      <c r="M15" s="20">
         <v>0</v>
       </c>
-      <c r="M15" s="6">
+      <c r="N15" s="21">
         <v>5</v>
       </c>
-      <c r="N15" s="6">
+      <c r="O15" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8302,44 +8424,47 @@
       <c r="A16" s="4">
         <v>14</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="9">
         <f>C15+1</f>
-        <v>201</v>
-      </c>
-      <c r="C16" s="5">
-        <v>300</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5">
-        <v>1</v>
-      </c>
-      <c r="F16" s="6">
-        <v>100</v>
-      </c>
-      <c r="G16" s="6">
+        <v>151</v>
+      </c>
+      <c r="C16" s="9">
+        <v>200</v>
+      </c>
+      <c r="D16" s="10">
         <v>2</v>
       </c>
-      <c r="H16" s="6">
-        <v>100</v>
-      </c>
-      <c r="I16" s="6">
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="11">
+        <v>1</v>
+      </c>
+      <c r="G16" s="17">
+        <v>100</v>
+      </c>
+      <c r="H16" s="18">
+        <v>2</v>
+      </c>
+      <c r="I16" s="18">
+        <v>100</v>
+      </c>
+      <c r="J16" s="19">
         <v>3</v>
       </c>
-      <c r="J16" s="6">
-        <v>100</v>
-      </c>
-      <c r="K16" s="6">
+      <c r="K16" s="19">
+        <v>100</v>
+      </c>
+      <c r="L16" s="20">
         <v>4</v>
       </c>
-      <c r="L16" s="6">
+      <c r="M16" s="20">
         <v>0</v>
       </c>
-      <c r="M16" s="6">
+      <c r="N16" s="21">
         <v>5</v>
       </c>
-      <c r="N16" s="6">
+      <c r="O16" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8347,44 +8472,47 @@
       <c r="A17" s="4">
         <v>15</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="9">
         <f>C16+1</f>
-        <v>301</v>
-      </c>
-      <c r="C17" s="5">
-        <v>400</v>
-      </c>
-      <c r="D17" s="5">
-        <v>19</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="6">
-        <v>100</v>
-      </c>
-      <c r="G17" s="6">
+        <v>201</v>
+      </c>
+      <c r="C17" s="9">
+        <v>300</v>
+      </c>
+      <c r="D17" s="10">
         <v>2</v>
       </c>
-      <c r="H17" s="6">
-        <v>100</v>
-      </c>
-      <c r="I17" s="6">
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="17">
+        <v>100</v>
+      </c>
+      <c r="H17" s="18">
+        <v>2</v>
+      </c>
+      <c r="I17" s="18">
+        <v>100</v>
+      </c>
+      <c r="J17" s="19">
         <v>3</v>
       </c>
-      <c r="J17" s="6">
-        <v>100</v>
-      </c>
-      <c r="K17" s="6">
+      <c r="K17" s="19">
+        <v>100</v>
+      </c>
+      <c r="L17" s="20">
         <v>4</v>
       </c>
-      <c r="L17" s="6">
+      <c r="M17" s="20">
         <v>0</v>
       </c>
-      <c r="M17" s="6">
+      <c r="N17" s="21">
         <v>5</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8392,44 +8520,47 @@
       <c r="A18" s="4">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="9">
         <f>C17+1</f>
-        <v>401</v>
-      </c>
-      <c r="C18" s="5">
-        <v>500</v>
-      </c>
-      <c r="D18" s="5">
-        <v>20</v>
-      </c>
-      <c r="E18" s="5">
-        <v>1</v>
-      </c>
-      <c r="F18" s="6">
-        <v>100</v>
-      </c>
-      <c r="G18" s="6">
+        <v>301</v>
+      </c>
+      <c r="C18" s="9">
+        <v>400</v>
+      </c>
+      <c r="D18" s="10">
         <v>2</v>
       </c>
-      <c r="H18" s="6">
-        <v>100</v>
-      </c>
-      <c r="I18" s="6">
+      <c r="E18" s="10">
+        <v>19</v>
+      </c>
+      <c r="F18" s="11">
+        <v>1</v>
+      </c>
+      <c r="G18" s="17">
+        <v>100</v>
+      </c>
+      <c r="H18" s="18">
+        <v>2</v>
+      </c>
+      <c r="I18" s="18">
+        <v>100</v>
+      </c>
+      <c r="J18" s="19">
         <v>3</v>
       </c>
-      <c r="J18" s="6">
-        <v>100</v>
-      </c>
-      <c r="K18" s="6">
+      <c r="K18" s="19">
+        <v>100</v>
+      </c>
+      <c r="L18" s="20">
         <v>4</v>
       </c>
-      <c r="L18" s="6">
+      <c r="M18" s="20">
         <v>0</v>
       </c>
-      <c r="M18" s="6">
+      <c r="N18" s="21">
         <v>5</v>
       </c>
-      <c r="N18" s="6">
+      <c r="O18" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8437,44 +8568,47 @@
       <c r="A19" s="4">
         <v>17</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="9">
         <f>C18+1</f>
-        <v>501</v>
-      </c>
-      <c r="C19" s="5">
-        <v>700</v>
-      </c>
-      <c r="D19" s="5">
-        <v>21</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="6">
-        <v>100</v>
-      </c>
-      <c r="G19" s="6">
+        <v>401</v>
+      </c>
+      <c r="C19" s="9">
+        <v>500</v>
+      </c>
+      <c r="D19" s="10">
         <v>2</v>
       </c>
-      <c r="H19" s="6">
-        <v>100</v>
-      </c>
-      <c r="I19" s="6">
+      <c r="E19" s="10">
+        <v>20</v>
+      </c>
+      <c r="F19" s="11">
+        <v>1</v>
+      </c>
+      <c r="G19" s="17">
+        <v>100</v>
+      </c>
+      <c r="H19" s="18">
+        <v>2</v>
+      </c>
+      <c r="I19" s="18">
+        <v>100</v>
+      </c>
+      <c r="J19" s="19">
         <v>3</v>
       </c>
-      <c r="J19" s="6">
-        <v>100</v>
-      </c>
-      <c r="K19" s="6">
+      <c r="K19" s="19">
+        <v>100</v>
+      </c>
+      <c r="L19" s="20">
         <v>4</v>
       </c>
-      <c r="L19" s="6">
+      <c r="M19" s="20">
         <v>0</v>
       </c>
-      <c r="M19" s="6">
+      <c r="N19" s="21">
         <v>5</v>
       </c>
-      <c r="N19" s="6">
+      <c r="O19" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8482,44 +8616,47 @@
       <c r="A20" s="4">
         <v>18</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="9">
         <f>C19+1</f>
-        <v>701</v>
-      </c>
-      <c r="C20" s="5">
-        <v>900</v>
-      </c>
-      <c r="D20" s="5">
-        <v>22</v>
-      </c>
-      <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="6">
-        <v>100</v>
-      </c>
-      <c r="G20" s="6">
+        <v>501</v>
+      </c>
+      <c r="C20" s="9">
+        <v>700</v>
+      </c>
+      <c r="D20" s="10">
         <v>2</v>
       </c>
-      <c r="H20" s="6">
-        <v>100</v>
-      </c>
-      <c r="I20" s="6">
+      <c r="E20" s="10">
+        <v>21</v>
+      </c>
+      <c r="F20" s="11">
+        <v>1</v>
+      </c>
+      <c r="G20" s="17">
+        <v>100</v>
+      </c>
+      <c r="H20" s="18">
+        <v>2</v>
+      </c>
+      <c r="I20" s="18">
+        <v>100</v>
+      </c>
+      <c r="J20" s="19">
         <v>3</v>
       </c>
-      <c r="J20" s="6">
-        <v>100</v>
-      </c>
-      <c r="K20" s="6">
+      <c r="K20" s="19">
+        <v>100</v>
+      </c>
+      <c r="L20" s="20">
         <v>4</v>
       </c>
-      <c r="L20" s="6">
+      <c r="M20" s="20">
         <v>0</v>
       </c>
-      <c r="M20" s="6">
+      <c r="N20" s="21">
         <v>5</v>
       </c>
-      <c r="N20" s="6">
+      <c r="O20" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8527,44 +8664,47 @@
       <c r="A21" s="4">
         <v>19</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="9">
         <f>C20+1</f>
-        <v>901</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1000</v>
-      </c>
-      <c r="D21" s="5">
-        <v>23</v>
-      </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21" s="6">
-        <v>100</v>
-      </c>
-      <c r="G21" s="6">
+        <v>701</v>
+      </c>
+      <c r="C21" s="9">
+        <v>900</v>
+      </c>
+      <c r="D21" s="10">
         <v>2</v>
       </c>
-      <c r="H21" s="6">
-        <v>100</v>
-      </c>
-      <c r="I21" s="6">
+      <c r="E21" s="10">
+        <v>22</v>
+      </c>
+      <c r="F21" s="11">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17">
+        <v>100</v>
+      </c>
+      <c r="H21" s="18">
+        <v>2</v>
+      </c>
+      <c r="I21" s="18">
+        <v>100</v>
+      </c>
+      <c r="J21" s="19">
         <v>3</v>
       </c>
-      <c r="J21" s="6">
-        <v>100</v>
-      </c>
-      <c r="K21" s="6">
+      <c r="K21" s="19">
+        <v>100</v>
+      </c>
+      <c r="L21" s="20">
         <v>4</v>
       </c>
-      <c r="L21" s="6">
+      <c r="M21" s="20">
         <v>0</v>
       </c>
-      <c r="M21" s="6">
+      <c r="N21" s="21">
         <v>5</v>
       </c>
-      <c r="N21" s="6">
+      <c r="O21" s="21">
         <v>0</v>
       </c>
     </row>
@@ -8572,44 +8712,95 @@
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="9">
         <f>C21+1</f>
+        <v>901</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="10">
+        <v>2</v>
+      </c>
+      <c r="E22" s="10">
+        <v>23</v>
+      </c>
+      <c r="F22" s="11">
+        <v>1</v>
+      </c>
+      <c r="G22" s="17">
+        <v>100</v>
+      </c>
+      <c r="H22" s="18">
+        <v>2</v>
+      </c>
+      <c r="I22" s="18">
+        <v>100</v>
+      </c>
+      <c r="J22" s="19">
+        <v>3</v>
+      </c>
+      <c r="K22" s="19">
+        <v>100</v>
+      </c>
+      <c r="L22" s="20">
+        <v>4</v>
+      </c>
+      <c r="M22" s="20">
+        <v>0</v>
+      </c>
+      <c r="N22" s="21">
+        <v>5</v>
+      </c>
+      <c r="O22" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1">
+      <c r="A23" s="4">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9">
+        <f>C22+1</f>
         <v>1001</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C23" s="9">
         <v>10000</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D23" s="10">
+        <v>2</v>
+      </c>
+      <c r="E23" s="10">
         <v>24</v>
       </c>
-      <c r="E22" s="5">
-        <v>1</v>
-      </c>
-      <c r="F22" s="6">
-        <v>100</v>
-      </c>
-      <c r="G22" s="6">
+      <c r="F23" s="11">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17">
+        <v>100</v>
+      </c>
+      <c r="H23" s="18">
         <v>2</v>
       </c>
-      <c r="H22" s="6">
-        <v>100</v>
-      </c>
-      <c r="I22" s="6">
+      <c r="I23" s="18">
+        <v>100</v>
+      </c>
+      <c r="J23" s="19">
         <v>3</v>
       </c>
-      <c r="J22" s="6">
-        <v>100</v>
-      </c>
-      <c r="K22" s="6">
+      <c r="K23" s="19">
+        <v>100</v>
+      </c>
+      <c r="L23" s="20">
         <v>4</v>
       </c>
-      <c r="L22" s="6">
+      <c r="M23" s="20">
         <v>0</v>
       </c>
-      <c r="M22" s="6">
+      <c r="N23" s="21">
         <v>5</v>
       </c>
-      <c r="N22" s="6"/>
+      <c r="O23" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed #199 FlixelRL-199 Floor4の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -8385,8 +8385,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="9">
-        <f>C4+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9">
         <v>6</v>
@@ -8395,7 +8394,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" t="s" s="11">
         <v>11</v>

</xml_diff>

<commit_message>
fixed #244 FlixelRL-244 Floor5の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -102,15 +102,33 @@
     <t>キラービー</t>
   </si>
   <si>
+    <t>SPECTER</t>
+  </si>
+  <si>
+    <t>specter</t>
+  </si>
+  <si>
+    <t>悪霊</t>
+  </si>
+  <si>
+    <t>亡霊</t>
+  </si>
+  <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>WAND6</t>
+  </si>
+  <si>
     <t>SKELETON_DOG</t>
   </si>
   <si>
     <t>skeleton_dog</t>
   </si>
   <si>
-    <t>悪霊</t>
-  </si>
-  <si>
     <t>がいこつ犬</t>
   </si>
   <si>
@@ -127,24 +145,6 @@
   </si>
   <si>
     <t>スケルトン</t>
-  </si>
-  <si>
-    <t>SPECTER</t>
-  </si>
-  <si>
-    <t>specter</t>
-  </si>
-  <si>
-    <t>亡霊</t>
-  </si>
-  <si>
-    <t>escape</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>WAND6</t>
   </si>
   <si>
     <t>GNOLE1</t>
@@ -1733,7 +1733,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1756,13 +1756,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1782,6 +1808,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -3350,45 +3382,51 @@
         <v>32</v>
       </c>
       <c r="E6" t="s" s="4">
+        <v>32</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s" s="4">
         <v>33</v>
       </c>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>100</v>
-      </c>
-      <c r="H6" s="5">
-        <v>40</v>
-      </c>
-      <c r="I6" s="5">
-        <v>5</v>
-      </c>
-      <c r="J6" s="5">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="5"/>
+      <c r="L6" t="s" s="4">
+        <v>34</v>
+      </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" t="s" s="4">
+        <v>35</v>
+      </c>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" t="s" s="3">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s" s="4">
         <v>31</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s" s="4">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -3397,13 +3435,13 @@
         <v>100</v>
       </c>
       <c r="H7" s="5">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="I7" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J7" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -3414,19 +3452,19 @@
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="s" s="3">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s" s="4">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s" s="4">
         <v>31</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s" s="4">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -3435,7 +3473,7 @@
         <v>100</v>
       </c>
       <c r="H8" s="5">
-        <v>160</v>
+        <v>80</v>
       </c>
       <c r="I8" s="5">
         <v>1</v>
@@ -3443,18 +3481,12 @@
       <c r="J8" s="5">
         <v>1</v>
       </c>
-      <c r="K8" t="s" s="4">
-        <v>41</v>
-      </c>
-      <c r="L8" t="s" s="4">
-        <v>42</v>
-      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" t="s" s="4">
-        <v>43</v>
-      </c>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" t="s" s="3">
@@ -3487,7 +3519,7 @@
       <c r="J9" s="5">
         <v>1</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="8"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="5"/>
@@ -8819,7 +8851,7 @@
       <c r="P149" s="5"/>
     </row>
     <row r="150" ht="20" customHeight="1">
-      <c r="A150" s="7"/>
+      <c r="A150" s="9"/>
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -8856,24 +8888,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="8" customWidth="1"/>
-    <col min="2" max="2" width="4" style="8" customWidth="1"/>
-    <col min="3" max="3" width="4.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="3.625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="3.5" style="8" customWidth="1"/>
-    <col min="6" max="6" width="3.5" style="8" customWidth="1"/>
-    <col min="7" max="7" width="2.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="3.25" style="8" customWidth="1"/>
-    <col min="9" max="9" width="3.625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="9.75" style="8" customWidth="1"/>
-    <col min="11" max="11" width="3.625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="3.125" style="8" customWidth="1"/>
-    <col min="13" max="13" width="3.625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="2.375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="3.625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="2.375" style="8" customWidth="1"/>
-    <col min="17" max="17" width="3.625" style="8" customWidth="1"/>
-    <col min="18" max="256" width="12.25" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="4" style="10" customWidth="1"/>
+    <col min="3" max="3" width="4.75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="3.625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="3.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="3.5" style="10" customWidth="1"/>
+    <col min="7" max="7" width="2.875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="10.8359" style="10" customWidth="1"/>
+    <col min="9" max="9" width="3.625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9.75" style="10" customWidth="1"/>
+    <col min="11" max="11" width="3.625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="3.125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="3.625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="2.375" style="10" customWidth="1"/>
+    <col min="15" max="15" width="3.625" style="10" customWidth="1"/>
+    <col min="16" max="16" width="2.375" style="10" customWidth="1"/>
+    <col min="17" max="17" width="3.625" style="10" customWidth="1"/>
+    <col min="18" max="256" width="12.25" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customHeight="1">
@@ -8933,52 +8965,52 @@
       <c r="A2" t="s" s="3">
         <v>16</v>
       </c>
-      <c r="B2" t="s" s="9">
+      <c r="B2" t="s" s="11">
         <v>16</v>
       </c>
-      <c r="C2" t="s" s="9">
+      <c r="C2" t="s" s="11">
         <v>16</v>
       </c>
-      <c r="D2" t="s" s="10">
+      <c r="D2" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="F2" t="s" s="10">
+      <c r="F2" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="G2" t="s" s="10">
+      <c r="G2" t="s" s="12">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="11">
+      <c r="H2" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="I2" t="s" s="11">
+      <c r="I2" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="J2" t="s" s="12">
+      <c r="J2" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="K2" t="s" s="12">
+      <c r="K2" t="s" s="14">
         <v>16</v>
       </c>
-      <c r="L2" t="s" s="13">
+      <c r="L2" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="M2" t="s" s="13">
+      <c r="M2" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="N2" t="s" s="14">
+      <c r="N2" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="O2" t="s" s="14">
+      <c r="O2" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="P2" t="s" s="15">
+      <c r="P2" t="s" s="17">
         <v>16</v>
       </c>
-      <c r="Q2" t="s" s="15">
+      <c r="Q2" t="s" s="17">
         <v>16</v>
       </c>
     </row>
@@ -8986,248 +9018,240 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
         <v>2</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="10">
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="12">
         <v>0</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
     </row>
     <row r="4" ht="20" customHeight="1">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="11">
         <f>C3+1</f>
         <v>2</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="11">
         <v>2</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="12">
         <v>2</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="10">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="12">
         <v>0</v>
       </c>
-      <c r="H4" t="s" s="11">
+      <c r="H4" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="I4" s="18">
-        <v>100</v>
-      </c>
-      <c r="J4" s="23"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
+      <c r="I4" s="20">
+        <v>100</v>
+      </c>
+      <c r="J4" s="25"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
     </row>
     <row r="5" ht="20" customHeight="1">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="11">
         <v>3</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="12">
         <v>2</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="12">
         <v>30</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" s="10">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s" s="11">
+      <c r="G5" s="12">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="I5" s="18">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s" s="12">
+      <c r="I5" s="20">
+        <v>100</v>
+      </c>
+      <c r="J5" t="s" s="14">
         <v>21</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="21">
         <v>50</v>
       </c>
-      <c r="L5" s="24"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
     </row>
     <row r="6" ht="20" customHeight="1">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <v>4</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="11">
         <v>4</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="12">
         <v>2</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="12">
         <v>30</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="12">
         <v>3</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="12">
         <v>2</v>
       </c>
-      <c r="H6" t="s" s="11">
+      <c r="H6" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="20">
         <v>30</v>
       </c>
-      <c r="J6" t="s" s="12">
+      <c r="J6" t="s" s="14">
         <v>21</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="21">
         <v>10</v>
       </c>
-      <c r="L6" t="s" s="13">
+      <c r="L6" t="s" s="15">
         <v>26</v>
       </c>
-      <c r="M6" s="20">
+      <c r="M6" s="22">
         <v>200</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
     </row>
     <row r="7" ht="20" customHeight="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="11">
         <f>C6+1</f>
         <v>5</v>
       </c>
-      <c r="C7" s="9">
-        <v>10</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="11">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12">
         <v>2</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="10">
-        <v>1</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1</v>
-      </c>
-      <c r="I7" s="18">
-        <v>100</v>
-      </c>
-      <c r="J7" s="19">
-        <v>2</v>
-      </c>
-      <c r="K7" s="19">
-        <v>100</v>
-      </c>
-      <c r="L7" s="20">
+      <c r="E7" s="12">
+        <v>30</v>
+      </c>
+      <c r="F7" s="12">
         <v>3</v>
       </c>
-      <c r="M7" s="20">
-        <v>100</v>
-      </c>
-      <c r="N7" s="21">
-        <v>4</v>
-      </c>
-      <c r="O7" s="21">
-        <v>0</v>
-      </c>
-      <c r="P7" s="22">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="22">
-        <v>0</v>
-      </c>
+      <c r="G7" s="12">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="I7" s="20">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s" s="14">
+        <v>29</v>
+      </c>
+      <c r="K7" s="21">
+        <v>100</v>
+      </c>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="11">
         <f>C7+1</f>
-        <v>11</v>
-      </c>
-      <c r="C8" s="9">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
         <v>15</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="12">
         <v>2</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1</v>
-      </c>
-      <c r="I8" s="18">
-        <v>100</v>
-      </c>
-      <c r="J8" s="19">
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="12">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>1</v>
+      </c>
+      <c r="I8" s="20">
+        <v>100</v>
+      </c>
+      <c r="J8" s="21">
         <v>2</v>
       </c>
-      <c r="K8" s="19">
-        <v>100</v>
-      </c>
-      <c r="L8" s="20">
+      <c r="K8" s="21">
+        <v>100</v>
+      </c>
+      <c r="L8" s="22">
         <v>3</v>
       </c>
-      <c r="M8" s="20">
-        <v>100</v>
-      </c>
-      <c r="N8" s="21">
+      <c r="M8" s="22">
+        <v>100</v>
+      </c>
+      <c r="N8" s="23">
         <v>4</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="23">
         <v>0</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="24">
         <v>5</v>
       </c>
-      <c r="Q8" s="22">
+      <c r="Q8" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9235,49 +9259,49 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="11">
         <f>C8+1</f>
         <v>16</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="11">
         <v>20</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>2</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="10">
-        <v>1</v>
-      </c>
-      <c r="H9" s="11">
-        <v>1</v>
-      </c>
-      <c r="I9" s="18">
-        <v>100</v>
-      </c>
-      <c r="J9" s="19">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="12">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>1</v>
+      </c>
+      <c r="I9" s="20">
+        <v>100</v>
+      </c>
+      <c r="J9" s="21">
         <v>2</v>
       </c>
-      <c r="K9" s="19">
-        <v>100</v>
-      </c>
-      <c r="L9" s="20">
+      <c r="K9" s="21">
+        <v>100</v>
+      </c>
+      <c r="L9" s="22">
         <v>3</v>
       </c>
-      <c r="M9" s="20">
-        <v>100</v>
-      </c>
-      <c r="N9" s="21">
+      <c r="M9" s="22">
+        <v>100</v>
+      </c>
+      <c r="N9" s="23">
         <v>4</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="23">
         <v>0</v>
       </c>
-      <c r="P9" s="22">
+      <c r="P9" s="24">
         <v>5</v>
       </c>
-      <c r="Q9" s="22">
+      <c r="Q9" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9285,49 +9309,49 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="11">
         <f>C9+1</f>
         <v>21</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="11">
         <v>30</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="12">
         <v>2</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="11">
-        <v>1</v>
-      </c>
-      <c r="I10" s="18">
-        <v>100</v>
-      </c>
-      <c r="J10" s="19">
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="12">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1</v>
+      </c>
+      <c r="I10" s="20">
+        <v>100</v>
+      </c>
+      <c r="J10" s="21">
         <v>2</v>
       </c>
-      <c r="K10" s="19">
-        <v>100</v>
-      </c>
-      <c r="L10" s="20">
+      <c r="K10" s="21">
+        <v>100</v>
+      </c>
+      <c r="L10" s="22">
         <v>3</v>
       </c>
-      <c r="M10" s="20">
-        <v>100</v>
-      </c>
-      <c r="N10" s="21">
+      <c r="M10" s="22">
+        <v>100</v>
+      </c>
+      <c r="N10" s="23">
         <v>4</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="23">
         <v>0</v>
       </c>
-      <c r="P10" s="22">
+      <c r="P10" s="24">
         <v>5</v>
       </c>
-      <c r="Q10" s="22">
+      <c r="Q10" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9335,49 +9359,49 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="11">
         <f>C10+1</f>
         <v>31</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="11">
         <v>40</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>2</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="10">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="18">
-        <v>100</v>
-      </c>
-      <c r="J11" s="19">
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="12">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>1</v>
+      </c>
+      <c r="I11" s="20">
+        <v>100</v>
+      </c>
+      <c r="J11" s="21">
         <v>2</v>
       </c>
-      <c r="K11" s="19">
-        <v>100</v>
-      </c>
-      <c r="L11" s="20">
+      <c r="K11" s="21">
+        <v>100</v>
+      </c>
+      <c r="L11" s="22">
         <v>3</v>
       </c>
-      <c r="M11" s="20">
-        <v>100</v>
-      </c>
-      <c r="N11" s="21">
+      <c r="M11" s="22">
+        <v>100</v>
+      </c>
+      <c r="N11" s="23">
         <v>4</v>
       </c>
-      <c r="O11" s="21">
+      <c r="O11" s="23">
         <v>0</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="24">
         <v>5</v>
       </c>
-      <c r="Q11" s="22">
+      <c r="Q11" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9385,49 +9409,49 @@
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="11">
         <f>C11+1</f>
         <v>41</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="11">
         <v>60</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="12">
         <v>2</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="10">
-        <v>1</v>
-      </c>
-      <c r="H12" s="11">
-        <v>1</v>
-      </c>
-      <c r="I12" s="18">
-        <v>100</v>
-      </c>
-      <c r="J12" s="19">
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="13">
+        <v>1</v>
+      </c>
+      <c r="I12" s="20">
+        <v>100</v>
+      </c>
+      <c r="J12" s="21">
         <v>2</v>
       </c>
-      <c r="K12" s="19">
-        <v>100</v>
-      </c>
-      <c r="L12" s="20">
+      <c r="K12" s="21">
+        <v>100</v>
+      </c>
+      <c r="L12" s="22">
         <v>3</v>
       </c>
-      <c r="M12" s="20">
-        <v>100</v>
-      </c>
-      <c r="N12" s="21">
+      <c r="M12" s="22">
+        <v>100</v>
+      </c>
+      <c r="N12" s="23">
         <v>4</v>
       </c>
-      <c r="O12" s="21">
+      <c r="O12" s="23">
         <v>0</v>
       </c>
-      <c r="P12" s="22">
+      <c r="P12" s="24">
         <v>5</v>
       </c>
-      <c r="Q12" s="22">
+      <c r="Q12" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9435,49 +9459,49 @@
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="11">
         <f>C12+1</f>
         <v>61</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="11">
         <v>80</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="12">
         <v>2</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
-      <c r="H13" s="11">
-        <v>1</v>
-      </c>
-      <c r="I13" s="18">
-        <v>100</v>
-      </c>
-      <c r="J13" s="19">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="12">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="20">
+        <v>100</v>
+      </c>
+      <c r="J13" s="21">
         <v>2</v>
       </c>
-      <c r="K13" s="19">
-        <v>100</v>
-      </c>
-      <c r="L13" s="20">
+      <c r="K13" s="21">
+        <v>100</v>
+      </c>
+      <c r="L13" s="22">
         <v>3</v>
       </c>
-      <c r="M13" s="20">
-        <v>100</v>
-      </c>
-      <c r="N13" s="21">
+      <c r="M13" s="22">
+        <v>100</v>
+      </c>
+      <c r="N13" s="23">
         <v>4</v>
       </c>
-      <c r="O13" s="21">
+      <c r="O13" s="23">
         <v>0</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="24">
         <v>5</v>
       </c>
-      <c r="Q13" s="22">
+      <c r="Q13" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9485,49 +9509,49 @@
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="11">
         <f>C13+1</f>
         <v>81</v>
       </c>
-      <c r="C14" s="9">
-        <v>100</v>
-      </c>
-      <c r="D14" s="10">
+      <c r="C14" s="11">
+        <v>100</v>
+      </c>
+      <c r="D14" s="12">
         <v>2</v>
       </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="10">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11">
-        <v>1</v>
-      </c>
-      <c r="I14" s="18">
-        <v>100</v>
-      </c>
-      <c r="J14" s="19">
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="12">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13">
+        <v>1</v>
+      </c>
+      <c r="I14" s="20">
+        <v>100</v>
+      </c>
+      <c r="J14" s="21">
         <v>2</v>
       </c>
-      <c r="K14" s="19">
-        <v>100</v>
-      </c>
-      <c r="L14" s="20">
+      <c r="K14" s="21">
+        <v>100</v>
+      </c>
+      <c r="L14" s="22">
         <v>3</v>
       </c>
-      <c r="M14" s="20">
-        <v>100</v>
-      </c>
-      <c r="N14" s="21">
+      <c r="M14" s="22">
+        <v>100</v>
+      </c>
+      <c r="N14" s="23">
         <v>4</v>
       </c>
-      <c r="O14" s="21">
+      <c r="O14" s="23">
         <v>0</v>
       </c>
-      <c r="P14" s="22">
+      <c r="P14" s="24">
         <v>5</v>
       </c>
-      <c r="Q14" s="22">
+      <c r="Q14" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9535,49 +9559,49 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="11">
         <f>C14+1</f>
         <v>101</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="11">
         <v>150</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="12">
         <v>2</v>
       </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="10">
-        <v>1</v>
-      </c>
-      <c r="H15" s="11">
-        <v>1</v>
-      </c>
-      <c r="I15" s="18">
-        <v>100</v>
-      </c>
-      <c r="J15" s="19">
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="12">
+        <v>1</v>
+      </c>
+      <c r="H15" s="13">
+        <v>1</v>
+      </c>
+      <c r="I15" s="20">
+        <v>100</v>
+      </c>
+      <c r="J15" s="21">
         <v>2</v>
       </c>
-      <c r="K15" s="19">
-        <v>100</v>
-      </c>
-      <c r="L15" s="20">
+      <c r="K15" s="21">
+        <v>100</v>
+      </c>
+      <c r="L15" s="22">
         <v>3</v>
       </c>
-      <c r="M15" s="20">
-        <v>100</v>
-      </c>
-      <c r="N15" s="21">
+      <c r="M15" s="22">
+        <v>100</v>
+      </c>
+      <c r="N15" s="23">
         <v>4</v>
       </c>
-      <c r="O15" s="21">
+      <c r="O15" s="23">
         <v>0</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="24">
         <v>5</v>
       </c>
-      <c r="Q15" s="22">
+      <c r="Q15" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9585,49 +9609,49 @@
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="11">
         <f>C15+1</f>
         <v>151</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="11">
         <v>200</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="12">
         <v>2</v>
       </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="10">
-        <v>1</v>
-      </c>
-      <c r="H16" s="11">
-        <v>1</v>
-      </c>
-      <c r="I16" s="18">
-        <v>100</v>
-      </c>
-      <c r="J16" s="19">
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
+      <c r="H16" s="13">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20">
+        <v>100</v>
+      </c>
+      <c r="J16" s="21">
         <v>2</v>
       </c>
-      <c r="K16" s="19">
-        <v>100</v>
-      </c>
-      <c r="L16" s="20">
+      <c r="K16" s="21">
+        <v>100</v>
+      </c>
+      <c r="L16" s="22">
         <v>3</v>
       </c>
-      <c r="M16" s="20">
-        <v>100</v>
-      </c>
-      <c r="N16" s="21">
+      <c r="M16" s="22">
+        <v>100</v>
+      </c>
+      <c r="N16" s="23">
         <v>4</v>
       </c>
-      <c r="O16" s="21">
+      <c r="O16" s="23">
         <v>0</v>
       </c>
-      <c r="P16" s="22">
+      <c r="P16" s="24">
         <v>5</v>
       </c>
-      <c r="Q16" s="22">
+      <c r="Q16" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9635,49 +9659,49 @@
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="11">
         <f>C16+1</f>
         <v>201</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="11">
         <v>300</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="12">
         <v>2</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="10">
-        <v>1</v>
-      </c>
-      <c r="H17" s="11">
-        <v>1</v>
-      </c>
-      <c r="I17" s="18">
-        <v>100</v>
-      </c>
-      <c r="J17" s="19">
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="12">
+        <v>1</v>
+      </c>
+      <c r="H17" s="13">
+        <v>1</v>
+      </c>
+      <c r="I17" s="20">
+        <v>100</v>
+      </c>
+      <c r="J17" s="21">
         <v>2</v>
       </c>
-      <c r="K17" s="19">
-        <v>100</v>
-      </c>
-      <c r="L17" s="20">
+      <c r="K17" s="21">
+        <v>100</v>
+      </c>
+      <c r="L17" s="22">
         <v>3</v>
       </c>
-      <c r="M17" s="20">
-        <v>100</v>
-      </c>
-      <c r="N17" s="21">
+      <c r="M17" s="22">
+        <v>100</v>
+      </c>
+      <c r="N17" s="23">
         <v>4</v>
       </c>
-      <c r="O17" s="21">
+      <c r="O17" s="23">
         <v>0</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="24">
         <v>5</v>
       </c>
-      <c r="Q17" s="22">
+      <c r="Q17" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9685,49 +9709,49 @@
       <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="11">
         <f>C17+1</f>
         <v>301</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="11">
         <v>400</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="12">
         <v>2</v>
       </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="10">
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="12">
         <v>19</v>
       </c>
-      <c r="H18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="18">
-        <v>100</v>
-      </c>
-      <c r="J18" s="19">
+      <c r="H18" s="13">
+        <v>1</v>
+      </c>
+      <c r="I18" s="20">
+        <v>100</v>
+      </c>
+      <c r="J18" s="21">
         <v>2</v>
       </c>
-      <c r="K18" s="19">
-        <v>100</v>
-      </c>
-      <c r="L18" s="20">
+      <c r="K18" s="21">
+        <v>100</v>
+      </c>
+      <c r="L18" s="22">
         <v>3</v>
       </c>
-      <c r="M18" s="20">
-        <v>100</v>
-      </c>
-      <c r="N18" s="21">
+      <c r="M18" s="22">
+        <v>100</v>
+      </c>
+      <c r="N18" s="23">
         <v>4</v>
       </c>
-      <c r="O18" s="21">
+      <c r="O18" s="23">
         <v>0</v>
       </c>
-      <c r="P18" s="22">
+      <c r="P18" s="24">
         <v>5</v>
       </c>
-      <c r="Q18" s="22">
+      <c r="Q18" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9735,49 +9759,49 @@
       <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="11">
         <f>C18+1</f>
         <v>401</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="11">
         <v>500</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="12">
         <v>2</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="10">
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="12">
         <v>20</v>
       </c>
-      <c r="H19" s="11">
-        <v>1</v>
-      </c>
-      <c r="I19" s="18">
-        <v>100</v>
-      </c>
-      <c r="J19" s="19">
+      <c r="H19" s="13">
+        <v>1</v>
+      </c>
+      <c r="I19" s="20">
+        <v>100</v>
+      </c>
+      <c r="J19" s="21">
         <v>2</v>
       </c>
-      <c r="K19" s="19">
-        <v>100</v>
-      </c>
-      <c r="L19" s="20">
+      <c r="K19" s="21">
+        <v>100</v>
+      </c>
+      <c r="L19" s="22">
         <v>3</v>
       </c>
-      <c r="M19" s="20">
-        <v>100</v>
-      </c>
-      <c r="N19" s="21">
+      <c r="M19" s="22">
+        <v>100</v>
+      </c>
+      <c r="N19" s="23">
         <v>4</v>
       </c>
-      <c r="O19" s="21">
+      <c r="O19" s="23">
         <v>0</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="24">
         <v>5</v>
       </c>
-      <c r="Q19" s="22">
+      <c r="Q19" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9785,49 +9809,49 @@
       <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="11">
         <f>C19+1</f>
         <v>501</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="11">
         <v>700</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="12">
         <v>2</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="10">
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="12">
         <v>21</v>
       </c>
-      <c r="H20" s="11">
-        <v>1</v>
-      </c>
-      <c r="I20" s="18">
-        <v>100</v>
-      </c>
-      <c r="J20" s="19">
+      <c r="H20" s="13">
+        <v>1</v>
+      </c>
+      <c r="I20" s="20">
+        <v>100</v>
+      </c>
+      <c r="J20" s="21">
         <v>2</v>
       </c>
-      <c r="K20" s="19">
-        <v>100</v>
-      </c>
-      <c r="L20" s="20">
+      <c r="K20" s="21">
+        <v>100</v>
+      </c>
+      <c r="L20" s="22">
         <v>3</v>
       </c>
-      <c r="M20" s="20">
-        <v>100</v>
-      </c>
-      <c r="N20" s="21">
+      <c r="M20" s="22">
+        <v>100</v>
+      </c>
+      <c r="N20" s="23">
         <v>4</v>
       </c>
-      <c r="O20" s="21">
+      <c r="O20" s="23">
         <v>0</v>
       </c>
-      <c r="P20" s="22">
+      <c r="P20" s="24">
         <v>5</v>
       </c>
-      <c r="Q20" s="22">
+      <c r="Q20" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9835,49 +9859,49 @@
       <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="11">
         <f>C20+1</f>
         <v>701</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="11">
         <v>900</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="12">
         <v>2</v>
       </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="10">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="12">
         <v>22</v>
       </c>
-      <c r="H21" s="11">
-        <v>1</v>
-      </c>
-      <c r="I21" s="18">
-        <v>100</v>
-      </c>
-      <c r="J21" s="19">
+      <c r="H21" s="13">
+        <v>1</v>
+      </c>
+      <c r="I21" s="20">
+        <v>100</v>
+      </c>
+      <c r="J21" s="21">
         <v>2</v>
       </c>
-      <c r="K21" s="19">
-        <v>100</v>
-      </c>
-      <c r="L21" s="20">
+      <c r="K21" s="21">
+        <v>100</v>
+      </c>
+      <c r="L21" s="22">
         <v>3</v>
       </c>
-      <c r="M21" s="20">
-        <v>100</v>
-      </c>
-      <c r="N21" s="21">
+      <c r="M21" s="22">
+        <v>100</v>
+      </c>
+      <c r="N21" s="23">
         <v>4</v>
       </c>
-      <c r="O21" s="21">
+      <c r="O21" s="23">
         <v>0</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="24">
         <v>5</v>
       </c>
-      <c r="Q21" s="22">
+      <c r="Q21" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9885,49 +9909,49 @@
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="11">
         <f>C21+1</f>
         <v>901</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="11">
         <v>1000</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="12">
         <v>2</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="10">
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="12">
         <v>23</v>
       </c>
-      <c r="H22" s="11">
-        <v>1</v>
-      </c>
-      <c r="I22" s="18">
-        <v>100</v>
-      </c>
-      <c r="J22" s="19">
+      <c r="H22" s="13">
+        <v>1</v>
+      </c>
+      <c r="I22" s="20">
+        <v>100</v>
+      </c>
+      <c r="J22" s="21">
         <v>2</v>
       </c>
-      <c r="K22" s="19">
-        <v>100</v>
-      </c>
-      <c r="L22" s="20">
+      <c r="K22" s="21">
+        <v>100</v>
+      </c>
+      <c r="L22" s="22">
         <v>3</v>
       </c>
-      <c r="M22" s="20">
-        <v>100</v>
-      </c>
-      <c r="N22" s="21">
+      <c r="M22" s="22">
+        <v>100</v>
+      </c>
+      <c r="N22" s="23">
         <v>4</v>
       </c>
-      <c r="O22" s="21">
+      <c r="O22" s="23">
         <v>0</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="24">
         <v>5</v>
       </c>
-      <c r="Q22" s="22">
+      <c r="Q22" s="24">
         <v>0</v>
       </c>
     </row>
@@ -9935,49 +9959,49 @@
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="11">
         <f>C22+1</f>
         <v>1001</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="11">
         <v>10000</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="12">
         <v>2</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="10">
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="12">
         <v>24</v>
       </c>
-      <c r="H23" s="11">
-        <v>1</v>
-      </c>
-      <c r="I23" s="18">
-        <v>100</v>
-      </c>
-      <c r="J23" s="19">
+      <c r="H23" s="13">
+        <v>1</v>
+      </c>
+      <c r="I23" s="20">
+        <v>100</v>
+      </c>
+      <c r="J23" s="21">
         <v>2</v>
       </c>
-      <c r="K23" s="19">
-        <v>100</v>
-      </c>
-      <c r="L23" s="20">
+      <c r="K23" s="21">
+        <v>100</v>
+      </c>
+      <c r="L23" s="22">
         <v>3</v>
       </c>
-      <c r="M23" s="20">
-        <v>100</v>
-      </c>
-      <c r="N23" s="21">
+      <c r="M23" s="22">
+        <v>100</v>
+      </c>
+      <c r="N23" s="23">
         <v>4</v>
       </c>
-      <c r="O23" s="21">
+      <c r="O23" s="23">
         <v>0</v>
       </c>
-      <c r="P23" s="22">
+      <c r="P23" s="24">
         <v>5</v>
       </c>
-      <c r="Q23" s="22"/>
+      <c r="Q23" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed #245 FlixelRL-245 Floor6の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -1762,7 +1762,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1837,6 +1837,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3398,16 +3401,16 @@
         <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="H7" s="5">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="I7" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="5"/>
@@ -3436,16 +3439,16 @@
         <v>1</v>
       </c>
       <c r="G8" s="4">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="H8" s="5">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="I8" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="5"/>
@@ -8863,13 +8866,13 @@
     <col min="5" max="5" width="3.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="3.5" style="8" customWidth="1"/>
     <col min="7" max="7" width="2.875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.8359" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9.75" style="8" customWidth="1"/>
     <col min="9" max="9" width="3.625" style="8" customWidth="1"/>
     <col min="10" max="10" width="9.75" style="8" customWidth="1"/>
     <col min="11" max="11" width="3.625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="3.125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="11" style="8" customWidth="1"/>
     <col min="13" max="13" width="3.625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="2.375" style="8" customWidth="1"/>
+    <col min="14" max="14" width="3.125" style="8" customWidth="1"/>
     <col min="15" max="15" width="3.625" style="8" customWidth="1"/>
     <col min="16" max="16" width="2.375" style="8" customWidth="1"/>
     <col min="17" max="17" width="3.625" style="8" customWidth="1"/>
@@ -9164,12 +9167,20 @@
         <v>29</v>
       </c>
       <c r="K7" s="19">
-        <v>100</v>
-      </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
+        <v>80</v>
+      </c>
+      <c r="L7" t="s" s="13">
+        <v>35</v>
+      </c>
+      <c r="M7" s="20">
+        <v>50</v>
+      </c>
+      <c r="N7" t="s" s="14">
+        <v>26</v>
+      </c>
+      <c r="O7" s="21">
+        <v>50</v>
+      </c>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
     </row>
@@ -9182,46 +9193,46 @@
         <v>6</v>
       </c>
       <c r="C8" s="9">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D8" s="10">
         <v>2</v>
       </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="E8" s="10">
+        <v>30</v>
+      </c>
+      <c r="F8" s="10">
+        <v>3</v>
+      </c>
       <c r="G8" s="10">
-        <v>1</v>
-      </c>
-      <c r="H8" s="11">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="H8" t="s" s="25">
+        <v>39</v>
       </c>
       <c r="I8" s="18">
-        <v>100</v>
-      </c>
-      <c r="J8" s="19">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="J8" t="s" s="12">
+        <v>29</v>
       </c>
       <c r="K8" s="19">
-        <v>100</v>
-      </c>
-      <c r="L8" s="20">
-        <v>3</v>
+        <v>70</v>
+      </c>
+      <c r="L8" t="s" s="13">
+        <v>35</v>
       </c>
       <c r="M8" s="20">
-        <v>100</v>
-      </c>
-      <c r="N8" s="21">
-        <v>4</v>
+        <v>50</v>
+      </c>
+      <c r="N8" t="s" s="14">
+        <v>26</v>
       </c>
       <c r="O8" s="21">
-        <v>0</v>
-      </c>
-      <c r="P8" s="22">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="22">
-        <v>0</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
     </row>
     <row r="9" ht="20" customHeight="1">
       <c r="A9" s="3">
@@ -9229,7 +9240,7 @@
       </c>
       <c r="B9" s="9">
         <f>C8+1</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C9" s="9">
         <v>20</v>

</xml_diff>

<commit_message>
fixed #429 FlixelRL-429 お金のドロップの設定
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="565">
   <si>
     <t>id</t>
   </si>
@@ -1532,6 +1532,9 @@
   </si>
   <si>
     <t>nightmare</t>
+  </si>
+  <si>
+    <t>MONEY</t>
   </si>
   <si>
     <t>INSECT_DEMON</t>
@@ -3235,7 +3238,7 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.55" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.19531" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.20312" style="1" customWidth="1"/>
     <col min="3" max="3" width="1.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9.57031" style="1" customWidth="1"/>
     <col min="5" max="5" width="5.61719" style="1" customWidth="1"/>
@@ -9995,8 +9998,12 @@
       <c r="O139" s="6"/>
       <c r="P139" s="6"/>
       <c r="Q139" s="6"/>
-      <c r="R139" s="6"/>
-      <c r="S139" s="6"/>
+      <c r="R139" t="s" s="5">
+        <v>506</v>
+      </c>
+      <c r="S139" s="6">
+        <v>100</v>
+      </c>
       <c r="T139" s="6"/>
       <c r="U139" s="6"/>
       <c r="V139" s="6"/>
@@ -10007,19 +10014,19 @@
     </row>
     <row r="140" ht="20" customHeight="1">
       <c r="A140" t="s" s="3">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B140" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C140" t="s" s="4">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D140" t="s" s="4">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E140" t="s" s="5">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F140" s="5">
         <v>3</v>
@@ -10055,19 +10062,19 @@
     </row>
     <row r="141" ht="20" customHeight="1">
       <c r="A141" t="s" s="3">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B141" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C141" t="s" s="4">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D141" t="s" s="4">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E141" t="s" s="5">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F141" s="5">
         <v>3</v>
@@ -10103,19 +10110,19 @@
     </row>
     <row r="142" ht="20" customHeight="1">
       <c r="A142" t="s" s="3">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B142" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C142" t="s" s="4">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="D142" t="s" s="4">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="E142" t="s" s="5">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F142" s="5">
         <v>4</v>
@@ -10151,19 +10158,19 @@
     </row>
     <row r="143" ht="20" customHeight="1">
       <c r="A143" t="s" s="3">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B143" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C143" t="s" s="4">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D143" t="s" s="4">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E143" t="s" s="5">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F143" s="5">
         <v>5</v>
@@ -10199,19 +10206,19 @@
     </row>
     <row r="144" ht="20" customHeight="1">
       <c r="A144" t="s" s="3">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B144" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C144" t="s" s="4">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D144" t="s" s="4">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E144" t="s" s="5">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="F144" s="5">
         <v>5</v>
@@ -10247,19 +10254,19 @@
     </row>
     <row r="145" ht="20" customHeight="1">
       <c r="A145" t="s" s="3">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B145" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C145" t="s" s="4">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D145" t="s" s="4">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E145" t="s" s="5">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F145" s="5">
         <v>5</v>
@@ -10295,19 +10302,19 @@
     </row>
     <row r="146" ht="20" customHeight="1">
       <c r="A146" t="s" s="3">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B146" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C146" t="s" s="4">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D146" t="s" s="4">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E146" t="s" s="5">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F146" s="5">
         <v>5</v>
@@ -10343,19 +10350,19 @@
     </row>
     <row r="147" ht="20" customHeight="1">
       <c r="A147" t="s" s="3">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B147" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C147" t="s" s="4">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D147" t="s" s="4">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E147" t="s" s="5">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="F147" s="5">
         <v>5</v>
@@ -10391,19 +10398,19 @@
     </row>
     <row r="148" ht="20" customHeight="1">
       <c r="A148" t="s" s="3">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B148" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C148" t="s" s="4">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D148" t="s" s="4">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E148" t="s" s="5">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F148" s="5">
         <v>5</v>
@@ -10439,19 +10446,19 @@
     </row>
     <row r="149" ht="20" customHeight="1">
       <c r="A149" t="s" s="3">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B149" t="s" s="4">
         <v>230</v>
       </c>
       <c r="C149" t="s" s="4">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D149" t="s" s="4">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E149" t="s" s="5">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="F149" s="5">
         <v>5</v>
@@ -10558,52 +10565,52 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -11689,16 +11696,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="2" ht="14.95" customHeight="1">
@@ -11732,7 +11739,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="4" ht="20" customHeight="1">
@@ -11740,7 +11747,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s" s="5">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="C4" s="5">
         <v>150</v>
@@ -11749,7 +11756,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s" s="5">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="5" ht="20" customHeight="1">
@@ -11757,7 +11764,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s" s="5">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C5" s="5">
         <v>160</v>
@@ -11766,7 +11773,7 @@
         <v>10</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="6" ht="20" customHeight="1">
@@ -11774,7 +11781,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="5">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C6" s="5">
         <v>165</v>
@@ -11783,7 +11790,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="s" s="5">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="7" ht="20" customHeight="1">
@@ -11791,7 +11798,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s" s="5">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C7" s="5">
         <v>170</v>
@@ -11800,7 +11807,7 @@
         <v>10</v>
       </c>
       <c r="E7" t="s" s="5">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="8" ht="20" customHeight="1">
@@ -11808,7 +11815,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C8" s="5">
         <v>50</v>
@@ -11817,7 +11824,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s" s="5">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="9" ht="20" customHeight="1">
@@ -11825,7 +11832,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C9" s="5">
         <v>120</v>
@@ -11834,7 +11841,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s" s="5">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="10" ht="20" customHeight="1">
@@ -11842,7 +11849,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="5">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C10" s="5">
         <v>140</v>
@@ -11851,7 +11858,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s" s="5">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="11" ht="20" customHeight="1">
@@ -11868,7 +11875,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s" s="5">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" ht="20" customHeight="1">
@@ -11885,7 +11892,7 @@
         <v>10</v>
       </c>
       <c r="E12" t="s" s="5">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="13" ht="20" customHeight="1">
@@ -11902,7 +11909,7 @@
         <v>10</v>
       </c>
       <c r="E13" t="s" s="5">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="14" ht="20" customHeight="1">
@@ -11919,7 +11926,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s" s="5">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1">
@@ -11936,7 +11943,7 @@
         <v>10</v>
       </c>
       <c r="E15" t="s" s="5">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -11953,7 +11960,7 @@
         <v>10</v>
       </c>
       <c r="E16" t="s" s="5">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed #246 FlixelRL-246 Floor7の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -10934,8 +10934,8 @@
       <c r="G9" s="16">
         <v>1</v>
       </c>
-      <c r="H9" s="17">
-        <v>1</v>
+      <c r="H9" t="s" s="17">
+        <v>25</v>
       </c>
       <c r="I9" s="24">
         <v>100</v>

</xml_diff>

<commit_message>
fixed #566 FlixelRL-566 Floor24〜26の敵の作成
</commit_message>
<xml_diff>
--- a/docs/enemy.xlsx
+++ b/docs/enemy.xlsx
@@ -451,10 +451,7 @@
     <t>ghost</t>
   </si>
   <si>
-    <t>WAND7</t>
-  </si>
-  <si>
-    <t>壁をすり抜ける。封印状態にする魔法を使う</t>
+    <t>WAND11</t>
   </si>
   <si>
     <t>DOG1</t>
@@ -520,6 +517,18 @@
     <t>ghoul</t>
   </si>
   <si>
+    <t>SHADOW_DEMON</t>
+  </si>
+  <si>
+    <t>影の悪魔</t>
+  </si>
+  <si>
+    <t>ナイトメアLv7</t>
+  </si>
+  <si>
+    <t>shadow_demon</t>
+  </si>
+  <si>
     <t>WRAITH</t>
   </si>
   <si>
@@ -1709,15 +1718,6 @@
   </si>
   <si>
     <t>hairy_demon</t>
-  </si>
-  <si>
-    <t>SHADOW_DEMON</t>
-  </si>
-  <si>
-    <t>影の悪魔</t>
-  </si>
-  <si>
-    <t>shadow_demon</t>
   </si>
   <si>
     <t>ICE_DEMON</t>
@@ -4779,10 +4779,12 @@
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" t="s" s="5">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="N24" s="7"/>
-      <c r="O24" s="6"/>
+      <c r="O24" t="s" s="5">
+        <v>55</v>
+      </c>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
@@ -4796,39 +4798,39 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
       <c r="Z24" t="s" s="5">
-        <v>146</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" ht="20" customHeight="1">
       <c r="A25" t="s" s="3">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C25" t="s" s="4">
+        <v>147</v>
+      </c>
+      <c r="D25" t="s" s="4">
         <v>148</v>
       </c>
-      <c r="D25" t="s" s="4">
+      <c r="E25" t="s" s="5">
         <v>149</v>
       </c>
-      <c r="E25" t="s" s="5">
+      <c r="F25" t="s" s="5">
         <v>150</v>
       </c>
-      <c r="F25" t="s" s="5">
-        <v>151</v>
-      </c>
       <c r="G25" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H25" s="6">
-        <v>550</v>
+        <v>8</v>
       </c>
       <c r="I25" s="6">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J25" s="6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -4836,7 +4838,7 @@
       <c r="N25" s="7"/>
       <c r="O25" s="6"/>
       <c r="P25" t="s" s="5">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q25" s="6">
         <v>20</v>
@@ -4850,30 +4852,30 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
       <c r="Z25" t="s" s="5">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" ht="20" customHeight="1">
       <c r="A26" t="s" s="8">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s" s="9">
         <v>43</v>
       </c>
       <c r="C26" t="s" s="9">
+        <v>154</v>
+      </c>
+      <c r="D26" t="s" s="9">
         <v>155</v>
       </c>
-      <c r="D26" t="s" s="9">
+      <c r="E26" t="s" s="10">
         <v>156</v>
-      </c>
-      <c r="E26" t="s" s="10">
-        <v>157</v>
       </c>
       <c r="F26" s="10">
         <v>5</v>
       </c>
       <c r="G26" s="10">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H26" s="11">
         <v>60</v>
@@ -4917,34 +4919,34 @@
     </row>
     <row r="27" ht="20" customHeight="1">
       <c r="A27" t="s" s="3">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B27" t="s" s="4">
         <v>52</v>
       </c>
       <c r="C27" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="D27" t="s" s="4">
+        <v>158</v>
+      </c>
+      <c r="E27" t="s" s="5">
         <v>159</v>
-      </c>
-      <c r="D27" t="s" s="4">
-        <v>159</v>
-      </c>
-      <c r="E27" t="s" s="5">
-        <v>160</v>
       </c>
       <c r="F27" s="5">
         <v>2</v>
       </c>
       <c r="G27" s="5">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="H27" s="6">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="I27" s="6">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="J27" s="6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
@@ -4967,34 +4969,34 @@
     </row>
     <row r="28" ht="20" customHeight="1">
       <c r="A28" t="s" s="3">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s" s="4">
         <v>52</v>
       </c>
       <c r="C28" t="s" s="4">
+        <v>161</v>
+      </c>
+      <c r="D28" t="s" s="4">
         <v>162</v>
       </c>
-      <c r="D28" t="s" s="4">
+      <c r="E28" t="s" s="5">
         <v>163</v>
-      </c>
-      <c r="E28" t="s" s="5">
-        <v>164</v>
       </c>
       <c r="F28" s="5">
         <v>2</v>
       </c>
       <c r="G28" s="5">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="H28" s="6">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="I28" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J28" s="6">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
@@ -5017,42 +5019,46 @@
     </row>
     <row r="29" ht="20" customHeight="1">
       <c r="A29" t="s" s="3">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B29" t="s" s="4">
         <v>52</v>
       </c>
       <c r="C29" t="s" s="4">
+        <v>165</v>
+      </c>
+      <c r="D29" t="s" s="4">
+        <v>165</v>
+      </c>
+      <c r="E29" t="s" s="5">
         <v>166</v>
-      </c>
-      <c r="D29" t="s" s="4">
-        <v>166</v>
-      </c>
-      <c r="E29" t="s" s="5">
-        <v>167</v>
       </c>
       <c r="F29" s="5">
         <v>2</v>
       </c>
       <c r="G29" s="5">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H29" s="6">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="I29" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J29" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
+      <c r="P29" t="s" s="5">
+        <v>108</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>20</v>
+      </c>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
@@ -5062,56 +5068,72 @@
       <c r="X29" s="6"/>
       <c r="Y29" s="6"/>
       <c r="Z29" t="s" s="5">
-        <v>50</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" ht="20" customHeight="1">
-      <c r="A30" t="s" s="3">
+      <c r="A30" t="s" s="8">
+        <v>167</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="C30" t="s" s="9">
         <v>168</v>
       </c>
-      <c r="B30" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="C30" t="s" s="4">
+      <c r="D30" t="s" s="9">
         <v>169</v>
       </c>
-      <c r="D30" t="s" s="4">
-        <v>169</v>
-      </c>
-      <c r="E30" t="s" s="5">
+      <c r="E30" t="s" s="10">
         <v>170</v>
       </c>
-      <c r="F30" s="5">
-        <v>2</v>
-      </c>
-      <c r="G30" s="5">
-        <v>100</v>
-      </c>
-      <c r="H30" s="6">
+      <c r="F30" s="10">
+        <v>5</v>
+      </c>
+      <c r="G30" s="10">
         <v>150</v>
       </c>
-      <c r="I30" s="6">
-        <v>1</v>
-      </c>
-      <c r="J30" s="6">
-        <v>1</v>
-      </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" t="s" s="5">
+      <c r="H30" s="11">
+        <v>60</v>
+      </c>
+      <c r="I30" s="11">
+        <v>25</v>
+      </c>
+      <c r="J30" s="11">
+        <v>25</v>
+      </c>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="14"/>
+      <c r="O30" t="s" s="10">
+        <v>55</v>
+      </c>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" t="s" s="10">
+        <v>145</v>
+      </c>
+      <c r="T30" t="s" s="10">
+        <v>47</v>
+      </c>
+      <c r="U30" s="11">
+        <v>100</v>
+      </c>
+      <c r="V30" t="s" s="10">
+        <v>48</v>
+      </c>
+      <c r="W30" s="11">
+        <v>50</v>
+      </c>
+      <c r="X30" t="s" s="10">
+        <v>49</v>
+      </c>
+      <c r="Y30" s="11">
+        <v>10</v>
+      </c>
+      <c r="Z30" t="s" s="10">
         <v>50</v>
       </c>
     </row>
@@ -5138,7 +5160,7 @@
         <v>100</v>
       </c>
       <c r="H31" s="6">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="I31" s="6">
         <v>1</v>
@@ -5176,10 +5198,10 @@
         <v>175</v>
       </c>
       <c r="D32" t="s" s="4">
+        <v>175</v>
+      </c>
+      <c r="E32" t="s" s="5">
         <v>176</v>
-      </c>
-      <c r="E32" t="s" s="5">
-        <v>177</v>
       </c>
       <c r="F32" s="5">
         <v>2</v>
@@ -5188,7 +5210,7 @@
         <v>100</v>
       </c>
       <c r="H32" s="6">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="I32" s="6">
         <v>1</v>
@@ -5217,13 +5239,13 @@
     </row>
     <row r="33" ht="20" customHeight="1">
       <c r="A33" t="s" s="3">
+        <v>177</v>
+      </c>
+      <c r="B33" t="s" s="4">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s" s="4">
         <v>178</v>
-      </c>
-      <c r="B33" t="s" s="4">
-        <v>78</v>
-      </c>
-      <c r="C33" t="s" s="4">
-        <v>179</v>
       </c>
       <c r="D33" t="s" s="4">
         <v>179</v>
@@ -5238,7 +5260,7 @@
         <v>100</v>
       </c>
       <c r="H33" s="6">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="I33" s="6">
         <v>1</v>
@@ -5276,10 +5298,10 @@
         <v>182</v>
       </c>
       <c r="D34" t="s" s="4">
+        <v>182</v>
+      </c>
+      <c r="E34" t="s" s="5">
         <v>183</v>
-      </c>
-      <c r="E34" t="s" s="5">
-        <v>184</v>
       </c>
       <c r="F34" s="5">
         <v>2</v>
@@ -5288,7 +5310,7 @@
         <v>100</v>
       </c>
       <c r="H34" s="6">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="I34" s="6">
         <v>1</v>
@@ -5317,19 +5339,19 @@
     </row>
     <row r="35" ht="20" customHeight="1">
       <c r="A35" t="s" s="3">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B35" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C35" t="s" s="4">
+        <v>185</v>
+      </c>
+      <c r="D35" t="s" s="4">
         <v>186</v>
       </c>
-      <c r="D35" t="s" s="4">
+      <c r="E35" t="s" s="5">
         <v>187</v>
-      </c>
-      <c r="E35" t="s" s="5">
-        <v>188</v>
       </c>
       <c r="F35" s="5">
         <v>2</v>
@@ -5338,7 +5360,7 @@
         <v>100</v>
       </c>
       <c r="H35" s="6">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="I35" s="6">
         <v>1</v>
@@ -5367,19 +5389,19 @@
     </row>
     <row r="36" ht="20" customHeight="1">
       <c r="A36" t="s" s="3">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B36" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C36" t="s" s="4">
+        <v>189</v>
+      </c>
+      <c r="D36" t="s" s="4">
         <v>190</v>
       </c>
-      <c r="D36" t="s" s="4">
+      <c r="E36" t="s" s="5">
         <v>191</v>
-      </c>
-      <c r="E36" t="s" s="5">
-        <v>192</v>
       </c>
       <c r="F36" s="5">
         <v>2</v>
@@ -5388,7 +5410,7 @@
         <v>100</v>
       </c>
       <c r="H36" s="6">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="I36" s="6">
         <v>1</v>
@@ -5417,19 +5439,19 @@
     </row>
     <row r="37" ht="20" customHeight="1">
       <c r="A37" t="s" s="3">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B37" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C37" t="s" s="4">
+        <v>193</v>
+      </c>
+      <c r="D37" t="s" s="4">
         <v>194</v>
       </c>
-      <c r="D37" t="s" s="4">
+      <c r="E37" t="s" s="5">
         <v>195</v>
-      </c>
-      <c r="E37" t="s" s="5">
-        <v>196</v>
       </c>
       <c r="F37" s="5">
         <v>2</v>
@@ -5438,7 +5460,7 @@
         <v>100</v>
       </c>
       <c r="H37" s="6">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="I37" s="6">
         <v>1</v>
@@ -5467,13 +5489,13 @@
     </row>
     <row r="38" ht="20" customHeight="1">
       <c r="A38" t="s" s="3">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B38" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C38" t="s" s="4">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D38" t="s" s="4">
         <v>198</v>
@@ -5488,7 +5510,7 @@
         <v>100</v>
       </c>
       <c r="H38" s="6">
-        <v>390</v>
+        <v>330</v>
       </c>
       <c r="I38" s="6">
         <v>1</v>
@@ -5538,7 +5560,7 @@
         <v>100</v>
       </c>
       <c r="H39" s="6">
-        <v>430</v>
+        <v>390</v>
       </c>
       <c r="I39" s="6">
         <v>1</v>
@@ -5570,7 +5592,7 @@
         <v>203</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s" s="4">
         <v>204</v>
@@ -5588,7 +5610,7 @@
         <v>100</v>
       </c>
       <c r="H40" s="6">
-        <v>790</v>
+        <v>430</v>
       </c>
       <c r="I40" s="6">
         <v>1</v>
@@ -5638,7 +5660,7 @@
         <v>100</v>
       </c>
       <c r="H41" s="6">
-        <v>810</v>
+        <v>790</v>
       </c>
       <c r="I41" s="6">
         <v>1</v>
@@ -5688,7 +5710,7 @@
         <v>100</v>
       </c>
       <c r="H42" s="6">
-        <v>820</v>
+        <v>810</v>
       </c>
       <c r="I42" s="6">
         <v>1</v>
@@ -5720,7 +5742,7 @@
         <v>212</v>
       </c>
       <c r="B43" t="s" s="4">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s" s="4">
         <v>213</v>
@@ -5732,26 +5754,26 @@
         <v>214</v>
       </c>
       <c r="F43" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H43" s="6">
-        <v>10</v>
+        <v>820</v>
       </c>
       <c r="I43" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J43" s="6">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
       <c r="N43" s="7"/>
       <c r="O43" s="6"/>
-      <c r="P43" s="7"/>
+      <c r="P43" s="6"/>
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
@@ -5762,7 +5784,7 @@
       <c r="X43" s="6"/>
       <c r="Y43" s="6"/>
       <c r="Z43" t="s" s="5">
-        <v>153</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" ht="20" customHeight="1">
@@ -5770,7 +5792,7 @@
         <v>215</v>
       </c>
       <c r="B44" t="s" s="4">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s" s="4">
         <v>216</v>
@@ -5782,26 +5804,26 @@
         <v>217</v>
       </c>
       <c r="F44" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G44" s="5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H44" s="6">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="I44" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J44" s="6">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
       <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
+      <c r="P44" s="7"/>
       <c r="Q44" s="6"/>
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
@@ -5812,7 +5834,7 @@
       <c r="X44" s="6"/>
       <c r="Y44" s="6"/>
       <c r="Z44" t="s" s="5">
-        <v>50</v>
+        <v>152</v>
       </c>
     </row>
     <row r="45" ht="20" customHeight="1">
@@ -5826,10 +5848,10 @@
         <v>219</v>
       </c>
       <c r="D45" t="s" s="4">
+        <v>219</v>
+      </c>
+      <c r="E45" t="s" s="5">
         <v>220</v>
-      </c>
-      <c r="E45" t="s" s="5">
-        <v>221</v>
       </c>
       <c r="F45" s="5">
         <v>3</v>
@@ -5838,7 +5860,7 @@
         <v>100</v>
       </c>
       <c r="H45" s="6">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I45" s="6">
         <v>1</v>
@@ -5867,13 +5889,13 @@
     </row>
     <row r="46" ht="20" customHeight="1">
       <c r="A46" t="s" s="3">
+        <v>221</v>
+      </c>
+      <c r="B46" t="s" s="4">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s" s="4">
         <v>222</v>
-      </c>
-      <c r="B46" t="s" s="4">
-        <v>78</v>
-      </c>
-      <c r="C46" t="s" s="4">
-        <v>223</v>
       </c>
       <c r="D46" t="s" s="4">
         <v>223</v>
@@ -5888,7 +5910,7 @@
         <v>100</v>
       </c>
       <c r="H46" s="6">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="I46" s="6">
         <v>1</v>
@@ -5926,10 +5948,10 @@
         <v>226</v>
       </c>
       <c r="D47" t="s" s="4">
+        <v>226</v>
+      </c>
+      <c r="E47" t="s" s="5">
         <v>227</v>
-      </c>
-      <c r="E47" t="s" s="5">
-        <v>228</v>
       </c>
       <c r="F47" s="5">
         <v>3</v>
@@ -5938,7 +5960,7 @@
         <v>100</v>
       </c>
       <c r="H47" s="6">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="I47" s="6">
         <v>1</v>
@@ -5967,19 +5989,19 @@
     </row>
     <row r="48" ht="20" customHeight="1">
       <c r="A48" t="s" s="3">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B48" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C48" t="s" s="4">
+        <v>229</v>
+      </c>
+      <c r="D48" t="s" s="4">
         <v>230</v>
       </c>
-      <c r="D48" t="s" s="4">
+      <c r="E48" t="s" s="5">
         <v>231</v>
-      </c>
-      <c r="E48" t="s" s="5">
-        <v>232</v>
       </c>
       <c r="F48" s="5">
         <v>3</v>
@@ -5988,7 +6010,7 @@
         <v>100</v>
       </c>
       <c r="H48" s="6">
-        <v>290</v>
+        <v>260</v>
       </c>
       <c r="I48" s="6">
         <v>1</v>
@@ -6017,19 +6039,19 @@
     </row>
     <row r="49" ht="20" customHeight="1">
       <c r="A49" t="s" s="3">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B49" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C49" t="s" s="4">
+        <v>233</v>
+      </c>
+      <c r="D49" t="s" s="4">
         <v>234</v>
       </c>
-      <c r="D49" t="s" s="4">
+      <c r="E49" t="s" s="5">
         <v>235</v>
-      </c>
-      <c r="E49" t="s" s="5">
-        <v>236</v>
       </c>
       <c r="F49" s="5">
         <v>3</v>
@@ -6038,7 +6060,7 @@
         <v>100</v>
       </c>
       <c r="H49" s="6">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="I49" s="6">
         <v>1</v>
@@ -6067,19 +6089,19 @@
     </row>
     <row r="50" ht="20" customHeight="1">
       <c r="A50" t="s" s="3">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B50" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C50" t="s" s="4">
+        <v>237</v>
+      </c>
+      <c r="D50" t="s" s="4">
         <v>238</v>
       </c>
-      <c r="D50" t="s" s="4">
+      <c r="E50" t="s" s="5">
         <v>239</v>
-      </c>
-      <c r="E50" t="s" s="5">
-        <v>240</v>
       </c>
       <c r="F50" s="5">
         <v>3</v>
@@ -6088,7 +6110,7 @@
         <v>100</v>
       </c>
       <c r="H50" s="6">
-        <v>340</v>
+        <v>310</v>
       </c>
       <c r="I50" s="6">
         <v>1</v>
@@ -6117,19 +6139,19 @@
     </row>
     <row r="51" ht="20" customHeight="1">
       <c r="A51" t="s" s="3">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B51" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C51" t="s" s="4">
+        <v>241</v>
+      </c>
+      <c r="D51" t="s" s="4">
         <v>242</v>
       </c>
-      <c r="D51" t="s" s="4">
+      <c r="E51" t="s" s="5">
         <v>243</v>
-      </c>
-      <c r="E51" t="s" s="5">
-        <v>244</v>
       </c>
       <c r="F51" s="5">
         <v>3</v>
@@ -6138,7 +6160,7 @@
         <v>100</v>
       </c>
       <c r="H51" s="6">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="I51" s="6">
         <v>1</v>
@@ -6167,13 +6189,13 @@
     </row>
     <row r="52" ht="20" customHeight="1">
       <c r="A52" t="s" s="3">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B52" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C52" t="s" s="4">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D52" t="s" s="4">
         <v>246</v>
@@ -6188,7 +6210,7 @@
         <v>100</v>
       </c>
       <c r="H52" s="6">
-        <v>400</v>
+        <v>360</v>
       </c>
       <c r="I52" s="6">
         <v>1</v>
@@ -6238,7 +6260,7 @@
         <v>100</v>
       </c>
       <c r="H53" s="6">
-        <v>420</v>
+        <v>400</v>
       </c>
       <c r="I53" s="6">
         <v>1</v>
@@ -6276,10 +6298,10 @@
         <v>252</v>
       </c>
       <c r="D54" t="s" s="4">
+        <v>252</v>
+      </c>
+      <c r="E54" t="s" s="5">
         <v>253</v>
-      </c>
-      <c r="E54" t="s" s="5">
-        <v>254</v>
       </c>
       <c r="F54" s="5">
         <v>3</v>
@@ -6288,7 +6310,7 @@
         <v>100</v>
       </c>
       <c r="H54" s="6">
-        <v>440</v>
+        <v>420</v>
       </c>
       <c r="I54" s="6">
         <v>1</v>
@@ -6317,19 +6339,19 @@
     </row>
     <row r="55" ht="20" customHeight="1">
       <c r="A55" t="s" s="3">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B55" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C55" t="s" s="4">
+        <v>255</v>
+      </c>
+      <c r="D55" t="s" s="4">
         <v>256</v>
       </c>
-      <c r="D55" t="s" s="4">
+      <c r="E55" t="s" s="5">
         <v>257</v>
-      </c>
-      <c r="E55" t="s" s="5">
-        <v>258</v>
       </c>
       <c r="F55" s="5">
         <v>3</v>
@@ -6338,7 +6360,7 @@
         <v>100</v>
       </c>
       <c r="H55" s="6">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="I55" s="6">
         <v>1</v>
@@ -6367,19 +6389,19 @@
     </row>
     <row r="56" ht="20" customHeight="1">
       <c r="A56" t="s" s="3">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B56" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C56" t="s" s="4">
+        <v>259</v>
+      </c>
+      <c r="D56" t="s" s="4">
         <v>260</v>
       </c>
-      <c r="D56" t="s" s="4">
+      <c r="E56" t="s" s="5">
         <v>261</v>
-      </c>
-      <c r="E56" t="s" s="5">
-        <v>262</v>
       </c>
       <c r="F56" s="5">
         <v>3</v>
@@ -6388,7 +6410,7 @@
         <v>100</v>
       </c>
       <c r="H56" s="6">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="I56" s="6">
         <v>1</v>
@@ -6417,13 +6439,13 @@
     </row>
     <row r="57" ht="20" customHeight="1">
       <c r="A57" t="s" s="3">
+        <v>262</v>
+      </c>
+      <c r="B57" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s" s="4">
         <v>263</v>
-      </c>
-      <c r="B57" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="C57" t="s" s="4">
-        <v>264</v>
       </c>
       <c r="D57" t="s" s="4">
         <v>264</v>
@@ -6432,16 +6454,16 @@
         <v>265</v>
       </c>
       <c r="F57" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G57" s="5">
         <v>100</v>
       </c>
       <c r="H57" s="6">
-        <v>10</v>
+        <v>460</v>
       </c>
       <c r="I57" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J57" s="6">
         <v>1</v>
@@ -6470,16 +6492,16 @@
         <v>266</v>
       </c>
       <c r="B58" t="s" s="4">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s" s="4">
         <v>267</v>
       </c>
       <c r="D58" t="s" s="4">
+        <v>267</v>
+      </c>
+      <c r="E58" t="s" s="5">
         <v>268</v>
-      </c>
-      <c r="E58" t="s" s="5">
-        <v>269</v>
       </c>
       <c r="F58" s="5">
         <v>4</v>
@@ -6488,10 +6510,10 @@
         <v>100</v>
       </c>
       <c r="H58" s="6">
-        <v>270</v>
+        <v>10</v>
       </c>
       <c r="I58" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J58" s="6">
         <v>1</v>
@@ -6517,19 +6539,19 @@
     </row>
     <row r="59" ht="20" customHeight="1">
       <c r="A59" t="s" s="3">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B59" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C59" t="s" s="4">
+        <v>270</v>
+      </c>
+      <c r="D59" t="s" s="4">
         <v>271</v>
       </c>
-      <c r="D59" t="s" s="4">
+      <c r="E59" t="s" s="5">
         <v>272</v>
-      </c>
-      <c r="E59" t="s" s="5">
-        <v>273</v>
       </c>
       <c r="F59" s="5">
         <v>4</v>
@@ -6538,7 +6560,7 @@
         <v>100</v>
       </c>
       <c r="H59" s="6">
-        <v>350</v>
+        <v>270</v>
       </c>
       <c r="I59" s="6">
         <v>1</v>
@@ -6567,13 +6589,13 @@
     </row>
     <row r="60" ht="20" customHeight="1">
       <c r="A60" t="s" s="3">
+        <v>273</v>
+      </c>
+      <c r="B60" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="C60" t="s" s="4">
         <v>274</v>
-      </c>
-      <c r="B60" t="s" s="4">
-        <v>52</v>
-      </c>
-      <c r="C60" t="s" s="4">
-        <v>275</v>
       </c>
       <c r="D60" t="s" s="4">
         <v>275</v>
@@ -6582,13 +6604,13 @@
         <v>276</v>
       </c>
       <c r="F60" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G60" s="5">
         <v>100</v>
       </c>
       <c r="H60" s="6">
-        <v>110</v>
+        <v>350</v>
       </c>
       <c r="I60" s="6">
         <v>1</v>
@@ -6638,7 +6660,7 @@
         <v>100</v>
       </c>
       <c r="H61" s="6">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="I61" s="6">
         <v>1</v>
@@ -6670,25 +6692,25 @@
         <v>280</v>
       </c>
       <c r="B62" t="s" s="4">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s" s="4">
         <v>281</v>
       </c>
       <c r="D62" t="s" s="4">
+        <v>281</v>
+      </c>
+      <c r="E62" t="s" s="5">
         <v>282</v>
       </c>
-      <c r="E62" t="s" s="5">
-        <v>283</v>
-      </c>
       <c r="F62" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G62" s="5">
         <v>100</v>
       </c>
       <c r="H62" s="6">
-        <v>370</v>
+        <v>140</v>
       </c>
       <c r="I62" s="6">
         <v>1</v>
@@ -6717,13 +6739,13 @@
     </row>
     <row r="63" ht="20" customHeight="1">
       <c r="A63" t="s" s="3">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B63" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C63" t="s" s="4">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D63" t="s" s="4">
         <v>285</v>
@@ -6738,7 +6760,7 @@
         <v>100</v>
       </c>
       <c r="H63" s="6">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="I63" s="6">
         <v>1</v>
@@ -6776,10 +6798,10 @@
         <v>288</v>
       </c>
       <c r="D64" t="s" s="4">
+        <v>288</v>
+      </c>
+      <c r="E64" t="s" s="5">
         <v>289</v>
-      </c>
-      <c r="E64" t="s" s="5">
-        <v>290</v>
       </c>
       <c r="F64" s="5">
         <v>4</v>
@@ -6788,7 +6810,7 @@
         <v>100</v>
       </c>
       <c r="H64" s="6">
-        <v>470</v>
+        <v>380</v>
       </c>
       <c r="I64" s="6">
         <v>1</v>
@@ -6817,19 +6839,19 @@
     </row>
     <row r="65" ht="20" customHeight="1">
       <c r="A65" t="s" s="3">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B65" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C65" t="s" s="4">
+        <v>291</v>
+      </c>
+      <c r="D65" t="s" s="4">
         <v>292</v>
       </c>
-      <c r="D65" t="s" s="4">
+      <c r="E65" t="s" s="5">
         <v>293</v>
-      </c>
-      <c r="E65" t="s" s="5">
-        <v>294</v>
       </c>
       <c r="F65" s="5">
         <v>4</v>
@@ -6838,7 +6860,7 @@
         <v>100</v>
       </c>
       <c r="H65" s="6">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="I65" s="6">
         <v>1</v>
@@ -6867,28 +6889,28 @@
     </row>
     <row r="66" ht="20" customHeight="1">
       <c r="A66" t="s" s="3">
+        <v>294</v>
+      </c>
+      <c r="B66" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="C66" t="s" s="4">
         <v>295</v>
       </c>
-      <c r="B66" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="C66" t="s" s="4">
+      <c r="D66" t="s" s="4">
         <v>296</v>
       </c>
-      <c r="D66" t="s" s="4">
+      <c r="E66" t="s" s="5">
         <v>297</v>
       </c>
-      <c r="E66" t="s" s="5">
-        <v>298</v>
-      </c>
       <c r="F66" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G66" s="5">
         <v>100</v>
       </c>
       <c r="H66" s="6">
-        <v>410</v>
+        <v>480</v>
       </c>
       <c r="I66" s="6">
         <v>1</v>
@@ -6917,13 +6939,13 @@
     </row>
     <row r="67" ht="20" customHeight="1">
       <c r="A67" t="s" s="3">
+        <v>298</v>
+      </c>
+      <c r="B67" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="C67" t="s" s="4">
         <v>299</v>
-      </c>
-      <c r="B67" t="s" s="4">
-        <v>78</v>
-      </c>
-      <c r="C67" t="s" s="4">
-        <v>300</v>
       </c>
       <c r="D67" t="s" s="4">
         <v>300</v>
@@ -6938,7 +6960,7 @@
         <v>100</v>
       </c>
       <c r="H67" s="6">
-        <v>490</v>
+        <v>410</v>
       </c>
       <c r="I67" s="6">
         <v>1</v>
@@ -6988,7 +7010,7 @@
         <v>100</v>
       </c>
       <c r="H68" s="6">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="I68" s="6">
         <v>1</v>
@@ -7038,7 +7060,7 @@
         <v>100</v>
       </c>
       <c r="H69" s="6">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="I69" s="6">
         <v>1</v>
@@ -7081,14 +7103,14 @@
       <c r="E70" t="s" s="5">
         <v>310</v>
       </c>
-      <c r="F70" t="s" s="5">
-        <v>151</v>
+      <c r="F70" s="5">
+        <v>5</v>
       </c>
       <c r="G70" s="5">
         <v>100</v>
       </c>
       <c r="H70" s="6">
-        <v>280</v>
+        <v>510</v>
       </c>
       <c r="I70" s="6">
         <v>1</v>
@@ -7120,25 +7142,25 @@
         <v>311</v>
       </c>
       <c r="B71" t="s" s="4">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="C71" t="s" s="4">
         <v>312</v>
       </c>
       <c r="D71" t="s" s="4">
+        <v>312</v>
+      </c>
+      <c r="E71" t="s" s="5">
         <v>313</v>
       </c>
-      <c r="E71" t="s" s="5">
-        <v>314</v>
-      </c>
       <c r="F71" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G71" s="5">
         <v>100</v>
       </c>
       <c r="H71" s="6">
-        <v>520</v>
+        <v>280</v>
       </c>
       <c r="I71" s="6">
         <v>1</v>
@@ -7167,28 +7189,28 @@
     </row>
     <row r="72" ht="20" customHeight="1">
       <c r="A72" t="s" s="3">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B72" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C72" t="s" s="4">
+        <v>315</v>
+      </c>
+      <c r="D72" t="s" s="4">
         <v>316</v>
       </c>
-      <c r="D72" t="s" s="4">
+      <c r="E72" t="s" s="5">
         <v>317</v>
       </c>
-      <c r="E72" t="s" s="5">
-        <v>318</v>
-      </c>
       <c r="F72" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G72" s="5">
         <v>100</v>
       </c>
       <c r="H72" s="6">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="I72" s="6">
         <v>1</v>
@@ -7217,28 +7239,28 @@
     </row>
     <row r="73" ht="20" customHeight="1">
       <c r="A73" t="s" s="3">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B73" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C73" t="s" s="4">
+        <v>319</v>
+      </c>
+      <c r="D73" t="s" s="4">
         <v>320</v>
       </c>
-      <c r="D73" t="s" s="4">
+      <c r="E73" t="s" s="5">
         <v>321</v>
       </c>
-      <c r="E73" t="s" s="5">
-        <v>322</v>
-      </c>
       <c r="F73" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G73" s="5">
         <v>100</v>
       </c>
       <c r="H73" s="6">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="I73" s="6">
         <v>1</v>
@@ -7267,28 +7289,28 @@
     </row>
     <row r="74" ht="20" customHeight="1">
       <c r="A74" t="s" s="3">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B74" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C74" t="s" s="4">
+        <v>323</v>
+      </c>
+      <c r="D74" t="s" s="4">
         <v>324</v>
       </c>
-      <c r="D74" t="s" s="4">
+      <c r="E74" t="s" s="5">
         <v>325</v>
       </c>
-      <c r="E74" t="s" s="5">
-        <v>326</v>
-      </c>
       <c r="F74" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G74" s="5">
         <v>100</v>
       </c>
       <c r="H74" s="6">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="I74" s="6">
         <v>1</v>
@@ -7317,13 +7339,13 @@
     </row>
     <row r="75" ht="20" customHeight="1">
       <c r="A75" t="s" s="3">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B75" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C75" t="s" s="4">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D75" t="s" s="4">
         <v>328</v>
@@ -7332,13 +7354,13 @@
         <v>329</v>
       </c>
       <c r="F75" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G75" s="5">
         <v>100</v>
       </c>
       <c r="H75" s="6">
-        <v>570</v>
+        <v>560</v>
       </c>
       <c r="I75" s="6">
         <v>1</v>
@@ -7382,13 +7404,13 @@
         <v>332</v>
       </c>
       <c r="F76" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G76" s="5">
         <v>100</v>
       </c>
       <c r="H76" s="6">
-        <v>580</v>
+        <v>570</v>
       </c>
       <c r="I76" s="6">
         <v>1</v>
@@ -7426,19 +7448,19 @@
         <v>334</v>
       </c>
       <c r="D77" t="s" s="4">
+        <v>334</v>
+      </c>
+      <c r="E77" t="s" s="5">
         <v>335</v>
       </c>
-      <c r="E77" t="s" s="5">
-        <v>336</v>
-      </c>
       <c r="F77" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G77" s="5">
         <v>100</v>
       </c>
       <c r="H77" s="6">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="I77" s="6">
         <v>1</v>
@@ -7467,13 +7489,13 @@
     </row>
     <row r="78" ht="20" customHeight="1">
       <c r="A78" t="s" s="3">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B78" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C78" t="s" s="4">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D78" t="s" s="4">
         <v>338</v>
@@ -7482,13 +7504,13 @@
         <v>339</v>
       </c>
       <c r="F78" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G78" s="5">
         <v>100</v>
       </c>
       <c r="H78" s="6">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="I78" s="6">
         <v>1</v>
@@ -7531,14 +7553,14 @@
       <c r="E79" t="s" s="5">
         <v>342</v>
       </c>
-      <c r="F79" s="5">
-        <v>3</v>
+      <c r="F79" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G79" s="5">
         <v>100</v>
       </c>
       <c r="H79" s="6">
-        <v>620</v>
+        <v>600</v>
       </c>
       <c r="I79" s="6">
         <v>1</v>
@@ -7582,13 +7604,13 @@
         <v>345</v>
       </c>
       <c r="F80" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G80" s="5">
         <v>100</v>
       </c>
       <c r="H80" s="6">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="I80" s="6">
         <v>1</v>
@@ -7632,13 +7654,13 @@
         <v>348</v>
       </c>
       <c r="F81" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G81" s="5">
         <v>100</v>
       </c>
       <c r="H81" s="6">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="I81" s="6">
         <v>1</v>
@@ -7688,7 +7710,7 @@
         <v>100</v>
       </c>
       <c r="H82" s="6">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="I82" s="6">
         <v>1</v>
@@ -7738,7 +7760,7 @@
         <v>100</v>
       </c>
       <c r="H83" s="6">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="I83" s="6">
         <v>1</v>
@@ -7782,13 +7804,13 @@
         <v>357</v>
       </c>
       <c r="F84" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G84" s="5">
         <v>100</v>
       </c>
       <c r="H84" s="6">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="I84" s="6">
         <v>1</v>
@@ -7838,7 +7860,7 @@
         <v>100</v>
       </c>
       <c r="H85" s="6">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="I85" s="6">
         <v>1</v>
@@ -7888,7 +7910,7 @@
         <v>100</v>
       </c>
       <c r="H86" s="6">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="I86" s="6">
         <v>1</v>
@@ -7938,7 +7960,7 @@
         <v>100</v>
       </c>
       <c r="H87" s="6">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="I87" s="6">
         <v>1</v>
@@ -7976,19 +7998,19 @@
         <v>368</v>
       </c>
       <c r="D88" t="s" s="4">
+        <v>368</v>
+      </c>
+      <c r="E88" t="s" s="5">
         <v>369</v>
       </c>
-      <c r="E88" t="s" s="5">
-        <v>370</v>
-      </c>
-      <c r="F88" t="s" s="5">
-        <v>151</v>
+      <c r="F88" s="5">
+        <v>3</v>
       </c>
       <c r="G88" s="5">
         <v>100</v>
       </c>
       <c r="H88" s="6">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="I88" s="6">
         <v>1</v>
@@ -8017,28 +8039,28 @@
     </row>
     <row r="89" ht="20" customHeight="1">
       <c r="A89" t="s" s="3">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B89" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C89" t="s" s="4">
+        <v>371</v>
+      </c>
+      <c r="D89" t="s" s="4">
         <v>372</v>
       </c>
-      <c r="D89" t="s" s="4">
+      <c r="E89" t="s" s="5">
         <v>373</v>
       </c>
-      <c r="E89" t="s" s="5">
-        <v>374</v>
-      </c>
       <c r="F89" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G89" s="5">
         <v>100</v>
       </c>
       <c r="H89" s="6">
-        <v>720</v>
+        <v>710</v>
       </c>
       <c r="I89" s="6">
         <v>1</v>
@@ -8067,28 +8089,28 @@
     </row>
     <row r="90" ht="20" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B90" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C90" t="s" s="4">
+        <v>375</v>
+      </c>
+      <c r="D90" t="s" s="4">
         <v>376</v>
       </c>
-      <c r="D90" t="s" s="4">
+      <c r="E90" t="s" s="5">
         <v>377</v>
       </c>
-      <c r="E90" t="s" s="5">
-        <v>378</v>
-      </c>
       <c r="F90" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G90" s="5">
         <v>100</v>
       </c>
       <c r="H90" s="6">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="I90" s="6">
         <v>1</v>
@@ -8117,28 +8139,28 @@
     </row>
     <row r="91" ht="20" customHeight="1">
       <c r="A91" t="s" s="3">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B91" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C91" t="s" s="4">
+        <v>379</v>
+      </c>
+      <c r="D91" t="s" s="4">
         <v>380</v>
       </c>
-      <c r="D91" t="s" s="4">
+      <c r="E91" t="s" s="5">
         <v>381</v>
       </c>
-      <c r="E91" t="s" s="5">
-        <v>382</v>
-      </c>
       <c r="F91" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G91" s="5">
         <v>100</v>
       </c>
       <c r="H91" s="6">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="I91" s="6">
         <v>1</v>
@@ -8167,13 +8189,13 @@
     </row>
     <row r="92" ht="20" customHeight="1">
       <c r="A92" t="s" s="3">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B92" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C92" t="s" s="4">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D92" t="s" s="4">
         <v>384</v>
@@ -8182,13 +8204,13 @@
         <v>385</v>
       </c>
       <c r="F92" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G92" s="5">
         <v>100</v>
       </c>
       <c r="H92" s="6">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="I92" s="6">
         <v>1</v>
@@ -8232,13 +8254,13 @@
         <v>388</v>
       </c>
       <c r="F93" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G93" s="5">
         <v>100</v>
       </c>
       <c r="H93" s="6">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="I93" s="6">
         <v>1</v>
@@ -8282,13 +8304,13 @@
         <v>391</v>
       </c>
       <c r="F94" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G94" s="5">
         <v>100</v>
       </c>
       <c r="H94" s="6">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="I94" s="6">
         <v>1</v>
@@ -8332,13 +8354,13 @@
         <v>394</v>
       </c>
       <c r="F95" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G95" s="5">
         <v>100</v>
       </c>
       <c r="H95" s="6">
-        <v>780</v>
+        <v>770</v>
       </c>
       <c r="I95" s="6">
         <v>1</v>
@@ -8381,14 +8403,14 @@
       <c r="E96" t="s" s="5">
         <v>397</v>
       </c>
-      <c r="F96" s="5">
-        <v>3</v>
+      <c r="F96" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G96" s="5">
         <v>100</v>
       </c>
       <c r="H96" s="6">
-        <v>830</v>
+        <v>780</v>
       </c>
       <c r="I96" s="6">
         <v>1</v>
@@ -8431,14 +8453,14 @@
       <c r="E97" t="s" s="5">
         <v>400</v>
       </c>
-      <c r="F97" t="s" s="5">
-        <v>151</v>
+      <c r="F97" s="5">
+        <v>3</v>
       </c>
       <c r="G97" s="5">
         <v>100</v>
       </c>
       <c r="H97" s="6">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="I97" s="6">
         <v>1</v>
@@ -8482,13 +8504,13 @@
         <v>403</v>
       </c>
       <c r="F98" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G98" s="5">
         <v>100</v>
       </c>
       <c r="H98" s="6">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="I98" s="6">
         <v>1</v>
@@ -8520,25 +8542,25 @@
         <v>404</v>
       </c>
       <c r="B99" t="s" s="4">
+        <v>28</v>
+      </c>
+      <c r="C99" t="s" s="4">
         <v>405</v>
       </c>
-      <c r="C99" t="s" s="4">
+      <c r="D99" t="s" s="4">
+        <v>405</v>
+      </c>
+      <c r="E99" t="s" s="5">
         <v>406</v>
       </c>
-      <c r="D99" t="s" s="4">
-        <v>407</v>
-      </c>
-      <c r="E99" t="s" s="5">
-        <v>408</v>
-      </c>
-      <c r="F99" s="5">
-        <v>2</v>
+      <c r="F99" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G99" s="5">
         <v>100</v>
       </c>
       <c r="H99" s="6">
-        <v>870</v>
+        <v>850</v>
       </c>
       <c r="I99" s="6">
         <v>1</v>
@@ -8567,13 +8589,13 @@
     </row>
     <row r="100" ht="20" customHeight="1">
       <c r="A100" t="s" s="3">
+        <v>407</v>
+      </c>
+      <c r="B100" t="s" s="4">
+        <v>408</v>
+      </c>
+      <c r="C100" t="s" s="4">
         <v>409</v>
-      </c>
-      <c r="B100" t="s" s="4">
-        <v>405</v>
-      </c>
-      <c r="C100" t="s" s="4">
-        <v>407</v>
       </c>
       <c r="D100" t="s" s="4">
         <v>410</v>
@@ -8588,7 +8610,7 @@
         <v>100</v>
       </c>
       <c r="H100" s="6">
-        <v>880</v>
+        <v>870</v>
       </c>
       <c r="I100" s="6">
         <v>1</v>
@@ -8620,10 +8642,10 @@
         <v>412</v>
       </c>
       <c r="B101" t="s" s="4">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C101" t="s" s="4">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D101" t="s" s="4">
         <v>413</v>
@@ -8631,14 +8653,14 @@
       <c r="E101" t="s" s="5">
         <v>414</v>
       </c>
-      <c r="F101" t="s" s="5">
-        <v>151</v>
+      <c r="F101" s="5">
+        <v>2</v>
       </c>
       <c r="G101" s="5">
         <v>100</v>
       </c>
       <c r="H101" s="6">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="I101" s="6">
         <v>1</v>
@@ -8670,7 +8692,7 @@
         <v>415</v>
       </c>
       <c r="B102" t="s" s="4">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C102" t="s" s="4">
         <v>416</v>
@@ -8682,13 +8704,13 @@
         <v>417</v>
       </c>
       <c r="F102" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G102" s="5">
         <v>100</v>
       </c>
       <c r="H102" s="6">
-        <v>900</v>
+        <v>890</v>
       </c>
       <c r="I102" s="6">
         <v>1</v>
@@ -8720,7 +8742,7 @@
         <v>418</v>
       </c>
       <c r="B103" t="s" s="4">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C103" t="s" s="4">
         <v>419</v>
@@ -8731,14 +8753,14 @@
       <c r="E103" t="s" s="5">
         <v>420</v>
       </c>
-      <c r="F103" s="5">
-        <v>4</v>
+      <c r="F103" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G103" s="5">
         <v>100</v>
       </c>
       <c r="H103" s="6">
-        <v>910</v>
+        <v>900</v>
       </c>
       <c r="I103" s="6">
         <v>1</v>
@@ -8770,7 +8792,7 @@
         <v>421</v>
       </c>
       <c r="B104" t="s" s="4">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C104" t="s" s="4">
         <v>422</v>
@@ -8782,13 +8804,13 @@
         <v>423</v>
       </c>
       <c r="F104" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G104" s="5">
         <v>100</v>
       </c>
       <c r="H104" s="6">
-        <v>920</v>
+        <v>910</v>
       </c>
       <c r="I104" s="6">
         <v>1</v>
@@ -8820,25 +8842,25 @@
         <v>424</v>
       </c>
       <c r="B105" t="s" s="4">
+        <v>408</v>
+      </c>
+      <c r="C105" t="s" s="4">
         <v>425</v>
       </c>
-      <c r="C105" t="s" s="4">
+      <c r="D105" t="s" s="4">
+        <v>425</v>
+      </c>
+      <c r="E105" t="s" s="5">
         <v>426</v>
       </c>
-      <c r="D105" t="s" s="4">
-        <v>426</v>
-      </c>
-      <c r="E105" t="s" s="5">
-        <v>427</v>
-      </c>
       <c r="F105" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G105" s="5">
         <v>100</v>
       </c>
       <c r="H105" s="6">
-        <v>930</v>
+        <v>920</v>
       </c>
       <c r="I105" s="6">
         <v>1</v>
@@ -8867,10 +8889,10 @@
     </row>
     <row r="106" ht="20" customHeight="1">
       <c r="A106" t="s" s="3">
+        <v>427</v>
+      </c>
+      <c r="B106" t="s" s="4">
         <v>428</v>
-      </c>
-      <c r="B106" t="s" s="4">
-        <v>425</v>
       </c>
       <c r="C106" t="s" s="4">
         <v>429</v>
@@ -8881,14 +8903,14 @@
       <c r="E106" t="s" s="5">
         <v>430</v>
       </c>
-      <c r="F106" t="s" s="5">
-        <v>151</v>
+      <c r="F106" s="5">
+        <v>2</v>
       </c>
       <c r="G106" s="5">
         <v>100</v>
       </c>
       <c r="H106" s="6">
-        <v>940</v>
+        <v>930</v>
       </c>
       <c r="I106" s="6">
         <v>1</v>
@@ -8920,25 +8942,25 @@
         <v>431</v>
       </c>
       <c r="B107" t="s" s="4">
+        <v>428</v>
+      </c>
+      <c r="C107" t="s" s="4">
         <v>432</v>
       </c>
-      <c r="C107" t="s" s="4">
+      <c r="D107" t="s" s="4">
+        <v>432</v>
+      </c>
+      <c r="E107" t="s" s="5">
         <v>433</v>
       </c>
-      <c r="D107" t="s" s="4">
-        <v>433</v>
-      </c>
-      <c r="E107" t="s" s="5">
-        <v>434</v>
-      </c>
-      <c r="F107" s="5">
-        <v>3</v>
+      <c r="F107" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G107" s="5">
         <v>100</v>
       </c>
       <c r="H107" s="6">
-        <v>950</v>
+        <v>940</v>
       </c>
       <c r="I107" s="6">
         <v>1</v>
@@ -8967,10 +8989,10 @@
     </row>
     <row r="108" ht="20" customHeight="1">
       <c r="A108" t="s" s="3">
+        <v>434</v>
+      </c>
+      <c r="B108" t="s" s="4">
         <v>435</v>
-      </c>
-      <c r="B108" t="s" s="4">
-        <v>432</v>
       </c>
       <c r="C108" t="s" s="4">
         <v>436</v>
@@ -8982,13 +9004,13 @@
         <v>437</v>
       </c>
       <c r="F108" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G108" s="5">
         <v>100</v>
       </c>
       <c r="H108" s="6">
-        <v>960</v>
+        <v>950</v>
       </c>
       <c r="I108" s="6">
         <v>1</v>
@@ -9020,7 +9042,7 @@
         <v>438</v>
       </c>
       <c r="B109" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C109" t="s" s="4">
         <v>439</v>
@@ -9038,7 +9060,7 @@
         <v>100</v>
       </c>
       <c r="H109" s="6">
-        <v>970</v>
+        <v>960</v>
       </c>
       <c r="I109" s="6">
         <v>1</v>
@@ -9070,7 +9092,7 @@
         <v>441</v>
       </c>
       <c r="B110" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C110" t="s" s="4">
         <v>442</v>
@@ -9082,13 +9104,13 @@
         <v>443</v>
       </c>
       <c r="F110" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G110" s="5">
         <v>100</v>
       </c>
       <c r="H110" s="6">
-        <v>980</v>
+        <v>970</v>
       </c>
       <c r="I110" s="6">
         <v>1</v>
@@ -9120,7 +9142,7 @@
         <v>444</v>
       </c>
       <c r="B111" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C111" t="s" s="4">
         <v>445</v>
@@ -9132,13 +9154,13 @@
         <v>446</v>
       </c>
       <c r="F111" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G111" s="5">
         <v>100</v>
       </c>
       <c r="H111" s="6">
-        <v>990</v>
+        <v>980</v>
       </c>
       <c r="I111" s="6">
         <v>1</v>
@@ -9170,7 +9192,7 @@
         <v>447</v>
       </c>
       <c r="B112" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C112" t="s" s="4">
         <v>448</v>
@@ -9188,7 +9210,7 @@
         <v>100</v>
       </c>
       <c r="H112" s="6">
-        <v>1000</v>
+        <v>990</v>
       </c>
       <c r="I112" s="6">
         <v>1</v>
@@ -9220,25 +9242,25 @@
         <v>450</v>
       </c>
       <c r="B113" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C113" t="s" s="4">
         <v>451</v>
       </c>
       <c r="D113" t="s" s="4">
+        <v>451</v>
+      </c>
+      <c r="E113" t="s" s="5">
         <v>452</v>
       </c>
-      <c r="E113" t="s" s="5">
-        <v>453</v>
-      </c>
       <c r="F113" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G113" s="5">
         <v>100</v>
       </c>
       <c r="H113" s="6">
-        <v>1010</v>
+        <v>1000</v>
       </c>
       <c r="I113" s="6">
         <v>1</v>
@@ -9267,19 +9289,19 @@
     </row>
     <row r="114" ht="20" customHeight="1">
       <c r="A114" t="s" s="3">
+        <v>453</v>
+      </c>
+      <c r="B114" t="s" s="4">
+        <v>435</v>
+      </c>
+      <c r="C114" t="s" s="4">
         <v>454</v>
       </c>
-      <c r="B114" t="s" s="4">
-        <v>432</v>
-      </c>
-      <c r="C114" t="s" s="4">
+      <c r="D114" t="s" s="4">
         <v>455</v>
       </c>
-      <c r="D114" t="s" s="4">
+      <c r="E114" t="s" s="5">
         <v>456</v>
-      </c>
-      <c r="E114" t="s" s="5">
-        <v>457</v>
       </c>
       <c r="F114" s="5">
         <v>4</v>
@@ -9288,7 +9310,7 @@
         <v>100</v>
       </c>
       <c r="H114" s="6">
-        <v>1020</v>
+        <v>1010</v>
       </c>
       <c r="I114" s="6">
         <v>1</v>
@@ -9317,13 +9339,13 @@
     </row>
     <row r="115" ht="20" customHeight="1">
       <c r="A115" t="s" s="3">
+        <v>457</v>
+      </c>
+      <c r="B115" t="s" s="4">
+        <v>435</v>
+      </c>
+      <c r="C115" t="s" s="4">
         <v>458</v>
-      </c>
-      <c r="B115" t="s" s="4">
-        <v>432</v>
-      </c>
-      <c r="C115" t="s" s="4">
-        <v>459</v>
       </c>
       <c r="D115" t="s" s="4">
         <v>459</v>
@@ -9332,13 +9354,13 @@
         <v>460</v>
       </c>
       <c r="F115" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G115" s="5">
         <v>100</v>
       </c>
       <c r="H115" s="6">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="I115" s="6">
         <v>1</v>
@@ -9370,7 +9392,7 @@
         <v>461</v>
       </c>
       <c r="B116" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C116" t="s" s="4">
         <v>462</v>
@@ -9388,7 +9410,7 @@
         <v>100</v>
       </c>
       <c r="H116" s="6">
-        <v>1040</v>
+        <v>1030</v>
       </c>
       <c r="I116" s="6">
         <v>1</v>
@@ -9420,7 +9442,7 @@
         <v>464</v>
       </c>
       <c r="B117" t="s" s="4">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C117" t="s" s="4">
         <v>465</v>
@@ -9431,14 +9453,14 @@
       <c r="E117" t="s" s="5">
         <v>466</v>
       </c>
-      <c r="F117" t="s" s="5">
-        <v>151</v>
+      <c r="F117" s="5">
+        <v>2</v>
       </c>
       <c r="G117" s="5">
         <v>100</v>
       </c>
       <c r="H117" s="6">
-        <v>1050</v>
+        <v>1040</v>
       </c>
       <c r="I117" s="6">
         <v>1</v>
@@ -9470,25 +9492,25 @@
         <v>467</v>
       </c>
       <c r="B118" t="s" s="4">
-        <v>33</v>
+        <v>435</v>
       </c>
       <c r="C118" t="s" s="4">
         <v>468</v>
       </c>
       <c r="D118" t="s" s="4">
+        <v>468</v>
+      </c>
+      <c r="E118" t="s" s="5">
         <v>469</v>
       </c>
-      <c r="E118" t="s" s="5">
-        <v>12</v>
-      </c>
       <c r="F118" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G118" s="5">
         <v>100</v>
       </c>
       <c r="H118" s="6">
-        <v>1060</v>
+        <v>1050</v>
       </c>
       <c r="I118" s="6">
         <v>1</v>
@@ -9526,19 +9548,19 @@
         <v>471</v>
       </c>
       <c r="D119" t="s" s="4">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E119" t="s" s="5">
-        <v>472</v>
-      </c>
-      <c r="F119" s="5">
-        <v>2</v>
+        <v>12</v>
+      </c>
+      <c r="F119" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G119" s="5">
         <v>100</v>
       </c>
       <c r="H119" s="6">
-        <v>1070</v>
+        <v>1060</v>
       </c>
       <c r="I119" s="6">
         <v>1</v>
@@ -9588,7 +9610,7 @@
         <v>100</v>
       </c>
       <c r="H120" s="6">
-        <v>1080</v>
+        <v>1070</v>
       </c>
       <c r="I120" s="6">
         <v>1</v>
@@ -9638,7 +9660,7 @@
         <v>100</v>
       </c>
       <c r="H121" s="6">
-        <v>1090</v>
+        <v>1080</v>
       </c>
       <c r="I121" s="6">
         <v>1</v>
@@ -9688,7 +9710,7 @@
         <v>100</v>
       </c>
       <c r="H122" s="6">
-        <v>1120</v>
+        <v>1090</v>
       </c>
       <c r="I122" s="6">
         <v>1</v>
@@ -9726,19 +9748,19 @@
         <v>483</v>
       </c>
       <c r="D123" t="s" s="4">
+        <v>483</v>
+      </c>
+      <c r="E123" t="s" s="5">
         <v>484</v>
       </c>
-      <c r="E123" t="s" s="5">
-        <v>485</v>
-      </c>
-      <c r="F123" t="s" s="5">
-        <v>151</v>
+      <c r="F123" s="5">
+        <v>2</v>
       </c>
       <c r="G123" s="5">
         <v>100</v>
       </c>
       <c r="H123" s="6">
-        <v>1130</v>
+        <v>1120</v>
       </c>
       <c r="I123" s="6">
         <v>1</v>
@@ -9767,13 +9789,13 @@
     </row>
     <row r="124" ht="20" customHeight="1">
       <c r="A124" t="s" s="3">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B124" t="s" s="4">
         <v>33</v>
       </c>
       <c r="C124" t="s" s="4">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D124" t="s" s="4">
         <v>487</v>
@@ -9782,13 +9804,13 @@
         <v>488</v>
       </c>
       <c r="F124" t="s" s="5">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G124" s="5">
         <v>100</v>
       </c>
       <c r="H124" s="6">
-        <v>1140</v>
+        <v>1130</v>
       </c>
       <c r="I124" s="6">
         <v>1</v>
@@ -9831,14 +9853,14 @@
       <c r="E125" t="s" s="5">
         <v>491</v>
       </c>
-      <c r="F125" s="5">
-        <v>2</v>
+      <c r="F125" t="s" s="5">
+        <v>150</v>
       </c>
       <c r="G125" s="5">
         <v>100</v>
       </c>
       <c r="H125" s="6">
-        <v>1160</v>
+        <v>1140</v>
       </c>
       <c r="I125" s="6">
         <v>1</v>
@@ -9882,13 +9904,13 @@
         <v>494</v>
       </c>
       <c r="F126" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G126" s="5">
         <v>100</v>
       </c>
       <c r="H126" s="6">
-        <v>1170</v>
+        <v>1160</v>
       </c>
       <c r="I126" s="6">
         <v>1</v>
@@ -9920,25 +9942,25 @@
         <v>495</v>
       </c>
       <c r="B127" t="s" s="4">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C127" t="s" s="4">
         <v>496</v>
       </c>
       <c r="D127" t="s" s="4">
+        <v>496</v>
+      </c>
+      <c r="E127" t="s" s="5">
         <v>497</v>
       </c>
-      <c r="E127" t="s" s="5">
-        <v>498</v>
-      </c>
       <c r="F127" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G127" s="5">
         <v>100</v>
       </c>
       <c r="H127" s="6">
-        <v>1180</v>
+        <v>1170</v>
       </c>
       <c r="I127" s="6">
         <v>1</v>
@@ -9967,28 +9989,28 @@
     </row>
     <row r="128" ht="20" customHeight="1">
       <c r="A128" t="s" s="3">
+        <v>498</v>
+      </c>
+      <c r="B128" t="s" s="4">
+        <v>43</v>
+      </c>
+      <c r="C128" t="s" s="4">
         <v>499</v>
       </c>
-      <c r="B128" t="s" s="4">
-        <v>122</v>
-      </c>
-      <c r="C128" t="s" s="4">
+      <c r="D128" t="s" s="4">
         <v>500</v>
       </c>
-      <c r="D128" t="s" s="4">
+      <c r="E128" t="s" s="5">
         <v>501</v>
       </c>
-      <c r="E128" t="s" s="5">
-        <v>502</v>
-      </c>
       <c r="F128" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G128" s="5">
         <v>100</v>
       </c>
       <c r="H128" s="6">
-        <v>1190</v>
+        <v>1180</v>
       </c>
       <c r="I128" s="6">
         <v>1</v>
@@ -10017,28 +10039,28 @@
     </row>
     <row r="129" ht="20" customHeight="1">
       <c r="A129" t="s" s="3">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B129" t="s" s="4">
         <v>122</v>
       </c>
       <c r="C129" t="s" s="4">
+        <v>503</v>
+      </c>
+      <c r="D129" t="s" s="4">
         <v>504</v>
       </c>
-      <c r="D129" t="s" s="4">
+      <c r="E129" t="s" s="5">
         <v>505</v>
       </c>
-      <c r="E129" t="s" s="5">
-        <v>506</v>
-      </c>
       <c r="F129" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G129" s="5">
         <v>100</v>
       </c>
       <c r="H129" s="6">
-        <v>1200</v>
+        <v>1190</v>
       </c>
       <c r="I129" s="6">
         <v>1</v>
@@ -10067,13 +10089,13 @@
     </row>
     <row r="130" ht="20" customHeight="1">
       <c r="A130" t="s" s="3">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B130" t="s" s="4">
         <v>122</v>
       </c>
       <c r="C130" t="s" s="4">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D130" t="s" s="4">
         <v>508</v>
@@ -10088,7 +10110,7 @@
         <v>100</v>
       </c>
       <c r="H130" s="6">
-        <v>1210</v>
+        <v>1200</v>
       </c>
       <c r="I130" s="6">
         <v>1</v>
@@ -10132,13 +10154,13 @@
         <v>512</v>
       </c>
       <c r="F131" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G131" s="5">
         <v>100</v>
       </c>
       <c r="H131" s="6">
-        <v>1220</v>
+        <v>1210</v>
       </c>
       <c r="I131" s="6">
         <v>1</v>
@@ -10182,13 +10204,13 @@
         <v>515</v>
       </c>
       <c r="F132" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G132" s="5">
         <v>100</v>
       </c>
       <c r="H132" s="6">
-        <v>1230</v>
+        <v>1220</v>
       </c>
       <c r="I132" s="6">
         <v>1</v>
@@ -10238,7 +10260,7 @@
         <v>100</v>
       </c>
       <c r="H133" s="6">
-        <v>1250</v>
+        <v>1230</v>
       </c>
       <c r="I133" s="6">
         <v>1</v>
@@ -10270,7 +10292,7 @@
         <v>519</v>
       </c>
       <c r="B134" t="s" s="4">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="C134" t="s" s="4">
         <v>520</v>
@@ -10288,7 +10310,7 @@
         <v>100</v>
       </c>
       <c r="H134" s="6">
-        <v>1260</v>
+        <v>1250</v>
       </c>
       <c r="I134" s="6">
         <v>1</v>
@@ -10320,7 +10342,7 @@
         <v>522</v>
       </c>
       <c r="B135" t="s" s="4">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C135" t="s" s="4">
         <v>523</v>
@@ -10332,13 +10354,13 @@
         <v>524</v>
       </c>
       <c r="F135" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G135" s="5">
         <v>100</v>
       </c>
       <c r="H135" s="6">
-        <v>1270</v>
+        <v>1260</v>
       </c>
       <c r="I135" s="6">
         <v>1</v>
@@ -10388,7 +10410,7 @@
         <v>100</v>
       </c>
       <c r="H136" s="6">
-        <v>1280</v>
+        <v>1270</v>
       </c>
       <c r="I136" s="6">
         <v>1</v>
@@ -10420,16 +10442,16 @@
         <v>528</v>
       </c>
       <c r="B137" t="s" s="4">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="C137" t="s" s="4">
         <v>529</v>
       </c>
       <c r="D137" t="s" s="4">
+        <v>529</v>
+      </c>
+      <c r="E137" t="s" s="5">
         <v>530</v>
-      </c>
-      <c r="E137" t="s" s="5">
-        <v>531</v>
       </c>
       <c r="F137" s="5">
         <v>3</v>
@@ -10438,7 +10460,7 @@
         <v>100</v>
       </c>
       <c r="H137" s="6">
-        <v>1290</v>
+        <v>1280</v>
       </c>
       <c r="I137" s="6">
         <v>1</v>
@@ -10467,19 +10489,19 @@
     </row>
     <row r="138" ht="20" customHeight="1">
       <c r="A138" t="s" s="3">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B138" t="s" s="4">
         <v>78</v>
       </c>
       <c r="C138" t="s" s="4">
+        <v>532</v>
+      </c>
+      <c r="D138" t="s" s="4">
         <v>533</v>
       </c>
-      <c r="D138" t="s" s="4">
+      <c r="E138" t="s" s="5">
         <v>534</v>
-      </c>
-      <c r="E138" t="s" s="5">
-        <v>535</v>
       </c>
       <c r="F138" s="5">
         <v>3</v>
@@ -10488,7 +10510,7 @@
         <v>100</v>
       </c>
       <c r="H138" s="6">
-        <v>1300</v>
+        <v>1290</v>
       </c>
       <c r="I138" s="6">
         <v>1</v>
@@ -10517,28 +10539,28 @@
     </row>
     <row r="139" ht="20" customHeight="1">
       <c r="A139" t="s" s="3">
+        <v>535</v>
+      </c>
+      <c r="B139" t="s" s="4">
+        <v>78</v>
+      </c>
+      <c r="C139" t="s" s="4">
         <v>536</v>
       </c>
-      <c r="B139" t="s" s="4">
-        <v>43</v>
-      </c>
-      <c r="C139" t="s" s="4">
+      <c r="D139" t="s" s="4">
         <v>537</v>
       </c>
-      <c r="D139" t="s" s="4">
+      <c r="E139" t="s" s="5">
         <v>538</v>
       </c>
-      <c r="E139" t="s" s="5">
-        <v>539</v>
-      </c>
       <c r="F139" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G139" s="5">
         <v>100</v>
       </c>
       <c r="H139" s="6">
-        <v>1310</v>
+        <v>1300</v>
       </c>
       <c r="I139" s="6">
         <v>1</v>
@@ -10548,8 +10570,8 @@
       </c>
       <c r="K139" s="7"/>
       <c r="L139" s="7"/>
-      <c r="M139" s="16"/>
-      <c r="N139" s="17"/>
+      <c r="M139" s="7"/>
+      <c r="N139" s="7"/>
       <c r="O139" s="6"/>
       <c r="P139" s="6"/>
       <c r="Q139" s="6"/>
@@ -10567,28 +10589,28 @@
     </row>
     <row r="140" ht="20" customHeight="1">
       <c r="A140" t="s" s="3">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B140" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C140" t="s" s="4">
+        <v>540</v>
+      </c>
+      <c r="D140" t="s" s="4">
         <v>541</v>
       </c>
-      <c r="D140" t="s" s="4">
+      <c r="E140" t="s" s="5">
         <v>542</v>
       </c>
-      <c r="E140" t="s" s="5">
-        <v>543</v>
-      </c>
       <c r="F140" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G140" s="5">
         <v>100</v>
       </c>
       <c r="H140" s="6">
-        <v>1320</v>
+        <v>1310</v>
       </c>
       <c r="I140" s="6">
         <v>1</v>
@@ -10617,13 +10639,13 @@
     </row>
     <row r="141" ht="20" customHeight="1">
       <c r="A141" t="s" s="3">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B141" t="s" s="4">
         <v>43</v>
       </c>
       <c r="C141" t="s" s="4">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D141" t="s" s="4">
         <v>545</v>
@@ -10632,13 +10654,13 @@
         <v>546</v>
       </c>
       <c r="F141" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G141" s="5">
         <v>100</v>
       </c>
       <c r="H141" s="6">
-        <v>1330</v>
+        <v>1320</v>
       </c>
       <c r="I141" s="6">
         <v>1</v>
@@ -10682,13 +10704,13 @@
         <v>549</v>
       </c>
       <c r="F142" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G142" s="5">
         <v>100</v>
       </c>
       <c r="H142" s="6">
-        <v>1340</v>
+        <v>1330</v>
       </c>
       <c r="I142" s="6">
         <v>1</v>
@@ -10732,13 +10754,13 @@
         <v>552</v>
       </c>
       <c r="F143" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G143" s="5">
         <v>100</v>
       </c>
       <c r="H143" s="6">
-        <v>1350</v>
+        <v>1340</v>
       </c>
       <c r="I143" s="6">
         <v>1</v>
@@ -10782,13 +10804,13 @@
         <v>555</v>
       </c>
       <c r="F144" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G144" s="5">
         <v>100</v>
       </c>
       <c r="H144" s="6">
-        <v>1360</v>
+        <v>1350</v>
       </c>
       <c r="I144" s="6">
         <v>1</v>
@@ -10832,19 +10854,19 @@
         <v>558</v>
       </c>
       <c r="F145" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G145" s="5">
         <v>100</v>
       </c>
       <c r="H145" s="6">
-        <v>30</v>
+        <v>1360</v>
       </c>
       <c r="I145" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J145" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K145" s="7"/>
       <c r="L145" s="7"/>
@@ -10932,7 +10954,7 @@
         <v>564</v>
       </c>
       <c r="F147" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G147" s="5">
         <v>100</v>
@@ -10982,7 +11004,7 @@
         <v>567</v>
       </c>
       <c r="F148" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G148" s="5">
         <v>100</v>
@@ -11798,7 +11820,7 @@
         <v>50</v>
       </c>
       <c r="L14" t="s" s="26">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M14" s="33">
         <v>100</v>
@@ -11822,30 +11844,50 @@
         <v>24</v>
       </c>
       <c r="C15" s="10">
-        <v>150</v>
+        <v>26</v>
       </c>
       <c r="D15" s="23">
         <v>2</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="E15" s="23">
+        <v>40</v>
+      </c>
+      <c r="F15" s="23">
+        <v>3</v>
+      </c>
       <c r="G15" s="23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" t="s" s="24">
-        <v>27</v>
+        <v>157</v>
       </c>
       <c r="I15" s="31">
         <v>100</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
+      <c r="J15" t="s" s="25">
+        <v>160</v>
+      </c>
+      <c r="K15" s="32">
+        <v>50</v>
+      </c>
+      <c r="L15" t="s" s="26">
+        <v>164</v>
+      </c>
+      <c r="M15" s="33">
+        <v>50</v>
+      </c>
+      <c r="N15" t="s" s="27">
+        <v>142</v>
+      </c>
+      <c r="O15" s="34">
+        <v>50</v>
+      </c>
+      <c r="P15" t="s" s="28">
+        <v>139</v>
+      </c>
+      <c r="Q15" s="35">
+        <v>20</v>
+      </c>
       <c r="R15" s="6"/>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -11854,7 +11896,7 @@
       </c>
       <c r="B16" s="10">
         <f>C15+1</f>
-        <v>151</v>
+        <v>27</v>
       </c>
       <c r="C16" s="10">
         <v>200</v>
@@ -12280,7 +12322,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s" s="5">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C8" s="5">
         <v>200</v>
@@ -12297,7 +12339,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s" s="5">
-        <v>565</v>
+        <v>167</v>
       </c>
       <c r="C9" s="5">
         <v>200</v>
@@ -12331,7 +12373,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s" s="5">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="C11" s="5">
         <v>200</v>
@@ -12348,7 +12390,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s" s="5">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="C12" s="5">
         <v>200</v>
@@ -12365,7 +12407,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s" s="5">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="C13" s="5">
         <v>200</v>
@@ -12382,7 +12424,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s" s="5">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="C14" s="5">
         <v>200</v>
@@ -12399,7 +12441,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s" s="5">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="C15" s="5">
         <v>200</v>
@@ -12416,7 +12458,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s" s="5">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="C16" s="5">
         <v>200</v>

</xml_diff>